<commit_message>
Laxman : Milk template rate chart
</commit_message>
<xml_diff>
--- a/Milk_Rate_Chart_Template.xlsx
+++ b/Milk_Rate_Chart_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Laxman\CSharp_Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Products\LPMilkDairyFirm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,32 +18,13 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -66,9 +47,21 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="8" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -93,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -101,7 +94,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -320,2122 +312,3001 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B3:R68"/>
+  <dimension ref="B3:R69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="4">
+      <c r="C3" s="1">
         <v>7.5</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="1">
         <v>7.6</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="1">
         <v>7.7</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="1">
         <v>7.8</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="1">
         <v>7.9</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="1">
         <v>8</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="1">
         <v>8.1</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="1">
         <v>8.1999999999999993</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="1">
         <v>8.3000000000000007</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="1">
         <v>8.4</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="1">
         <v>8.5</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>18</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>18.3</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>18.600000000000001</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <v>18.899999999999999</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="4">
         <v>19.2</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="4">
         <v>19.5</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="4">
         <v>19.7</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="4">
         <v>19.899999999999999</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="4">
         <v>20.3</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="4">
         <v>20.5</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4">
+      <c r="B5" s="1">
         <v>3.1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>18.3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>18.600000000000001</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>18.899999999999999</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="4">
         <v>19.2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <v>19.5</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="4">
         <v>19.8</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="4">
         <v>20</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="4">
         <v>20.2</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="4">
         <v>20.6</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
         <v>20.8</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>3.2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>18.600000000000001</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>18.899999999999999</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>19.2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>19.5</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="4">
         <v>19.8</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="4">
         <v>20.3</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="4">
         <v>20.5</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="4">
         <v>20.7</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="4">
         <v>20.9</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="4">
         <v>21.1</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>3.3</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>18.899999999999999</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>19.2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <v>19.5</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
         <v>19.8</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="4">
         <v>20.6</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="4">
         <v>20.8</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="4">
         <v>21</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="4">
         <v>21.2</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="4">
         <v>21.4</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>3.4</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>19.2</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>19.5</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>19.8</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="4">
         <v>20.7</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="4">
         <v>20.9</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="4">
         <v>21.1</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="4">
         <v>21.3</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="4">
         <v>21.5</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="4">
         <v>21.7</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>3.5000000000000102</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>19.5</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>19.8</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="4">
         <v>20.7</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="4">
         <v>21</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="4">
         <v>21.2</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="4">
         <v>21.4</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="4">
         <v>21.6</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="4">
         <v>21.8</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="4">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>3.6000000000000099</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>19.600000000000001</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>19.899999999999999</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>20.2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="4">
         <v>20.5</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="4">
         <v>20.8</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="4">
         <v>21.1</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="4">
         <v>21.3</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="4">
         <v>21.5</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="4">
         <v>21.7</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="4">
         <v>21.9</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="4">
         <v>22.1</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="4">
+      <c r="B11" s="1">
         <v>3.7000000000000099</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>19.7</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>20</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>20.3</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="4">
         <v>20.6</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="4">
         <v>20.9</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="4">
         <v>21.2</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="4">
         <v>21.4</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="4">
         <v>21.6</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="4">
         <v>21.8</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="4">
         <v>22</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="4">
         <v>22.2</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="4">
+      <c r="B12" s="1">
         <v>3.80000000000001</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>19.8</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="4">
         <v>20.7</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="4">
         <v>21</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="4">
         <v>21.3</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="4">
         <v>21.5</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="4">
         <v>21.7</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="4">
         <v>21.9</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="4">
         <v>22.1</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="4">
         <v>22.3</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4">
+      <c r="B13" s="1">
         <v>3.9000000000000101</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <v>19.899999999999999</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="4">
         <v>20.2</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="4">
         <v>20.5</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="4">
         <v>20.8</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="4">
         <v>21.1</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="4">
         <v>21.4</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="4">
         <v>21.6</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="4">
         <v>21.8</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="4">
         <v>22</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="4">
         <v>22.2</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="4">
         <v>22.4</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="4">
+      <c r="B14" s="1">
         <v>4.0000000000000098</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <v>20</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <v>20.3</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <v>20.6</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="4">
         <v>20.9</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="4">
         <v>21.2</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="4">
         <v>21.5</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="4">
         <v>21.7</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="4">
         <v>21.9</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="4">
         <v>22.1</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="4">
         <v>22.3</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="4">
         <v>22.5</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="4">
+      <c r="B15" s="1">
         <v>4.1000000000000103</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <v>20.7</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="4">
         <v>21</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="4">
         <v>21.3</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="4">
         <v>21.6</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="4">
         <v>21.8</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="4">
         <v>22</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="4">
         <v>22.2</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="4">
         <v>22.4</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="4">
         <v>22.6</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="4">
+      <c r="B16" s="1">
         <v>4.2000000000000099</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <v>20.2</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>20.5</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>20.8</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="4">
         <v>21.1</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="4">
         <v>21.4</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <v>21.7</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="4">
         <v>21.9</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="4">
         <v>22.1</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="4">
         <v>22.3</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="4">
         <v>22.5</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="4">
         <v>22.7</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="4">
+      <c r="B17" s="1">
         <v>4.3000000000000096</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <v>20.3</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>20.6</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>20.9</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="4">
         <v>21.2</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="4">
         <v>21.5</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="4">
         <v>21.8</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="4">
         <v>22</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="4">
         <v>22.2</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="4">
         <v>22.4</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="4">
         <v>22.6</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="4">
         <v>22.8</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B18" s="4">
+      <c r="B18" s="1">
         <v>4.4000000000000101</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="4">
         <v>20.7</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>21</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="4">
         <v>21.3</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="4">
         <v>21.6</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="4">
         <v>21.9</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="4">
         <v>22.1</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="4">
         <v>22.3</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="4">
         <v>22.5</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18" s="4">
         <v>22.7</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M18" s="4">
         <v>22.9</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B19" s="4">
+      <c r="B19" s="1">
         <v>4.5000000000000204</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="4">
         <v>20.5</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="4">
         <v>20.8</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="4">
         <v>21.1</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="4">
         <v>21.4</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="4">
         <v>21.7</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="4">
         <v>22</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="4">
         <v>22.2</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="4">
         <v>22.4</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="4">
         <v>22.6</v>
       </c>
-      <c r="L19" s="1">
+      <c r="L19" s="4">
         <v>22.8</v>
       </c>
-      <c r="M19" s="1">
+      <c r="M19" s="4">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B20" s="4">
+      <c r="B20" s="1">
         <v>4.6000000000000201</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="4">
         <v>20.6</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="4">
         <v>20.9</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="4">
         <v>21.2</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="4">
         <v>21.5</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="4">
         <v>21.8</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="4">
         <v>22.1</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="4">
         <v>22.3</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="4">
         <v>22.5</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="4">
         <v>22.7</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L20" s="4">
         <v>22.9</v>
       </c>
-      <c r="M20" s="1">
+      <c r="M20" s="4">
         <v>23.1</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B21" s="4">
+      <c r="B21" s="1">
         <v>4.7000000000000197</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="4">
         <v>20.7</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="4">
         <v>21</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="4">
         <v>21.3</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="4">
         <v>21.6</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="4">
         <v>21.9</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="4">
         <v>22.2</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="4">
         <v>22.4</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="4">
         <v>22.6</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="4">
         <v>22.8</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L21" s="4">
         <v>23</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M21" s="4">
         <v>23.2</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B22" s="4">
+      <c r="B22" s="1">
         <v>4.8000000000000203</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="4">
         <v>20.8</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="4">
         <v>21.1</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="4">
         <v>21.4</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="4">
         <v>21.7</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="4">
         <v>22</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="4">
         <v>22.3</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="4">
         <v>22.5</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="4">
         <v>22.7</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="4">
         <v>22.9</v>
       </c>
-      <c r="L22" s="1">
+      <c r="L22" s="4">
         <v>23.1</v>
       </c>
-      <c r="M22" s="1">
+      <c r="M22" s="4">
         <v>23.3</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B23" s="4">
+      <c r="B23" s="1">
         <v>4.9000000000000199</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="4">
         <v>20.9</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="4">
         <v>21.2</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="4">
         <v>21.5</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="4">
         <v>21.8</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="4">
         <v>22.1</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="4">
         <v>22.4</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="4">
         <v>22.6</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="4">
         <v>22.8</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="4">
         <v>23</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L23" s="4">
         <v>23.2</v>
       </c>
-      <c r="M23" s="1">
+      <c r="M23" s="4">
         <v>23.4</v>
       </c>
     </row>
     <row r="24" spans="2:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B24" s="4">
+      <c r="B24" s="1">
         <v>5.0000000000000204</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="4">
         <v>21</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="4">
         <v>21.3</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="4">
         <v>21.6</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="4">
         <v>21.9</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="4">
         <v>22.2</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="4">
         <v>22.5</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="4">
         <v>22.7</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="4">
         <v>22.9</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="4">
         <v>23.1</v>
       </c>
-      <c r="L24" s="1">
+      <c r="L24" s="4">
         <v>23.3</v>
       </c>
-      <c r="M24" s="1">
+      <c r="M24" s="4">
         <v>23.5</v>
       </c>
     </row>
     <row r="25" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="4">
+      <c r="B25" s="1">
         <v>5.1000000000000201</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="4">
         <v>21.1</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="4">
         <v>21.4</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="4">
         <v>21.7</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="4">
         <v>22</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="4">
         <v>22.3</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="4">
         <v>22.6</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="4">
         <v>22.8</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="4">
         <v>23</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="4">
         <v>23.2</v>
       </c>
-      <c r="L25" s="1">
+      <c r="L25" s="4">
         <v>23.4</v>
       </c>
-      <c r="M25" s="1">
+      <c r="M25" s="4">
         <v>23.6</v>
       </c>
     </row>
     <row r="26" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="4">
+      <c r="B26" s="1">
         <v>5.2000000000000197</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="4">
         <v>21.2</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="4">
         <v>21.5</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="4">
         <v>21.8</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="4">
         <v>22.1</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="4">
         <v>22.4</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="4">
         <v>22.7</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="4">
         <v>22.9</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="4">
         <v>23.1</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26" s="4">
         <v>23.3</v>
       </c>
-      <c r="L26" s="1">
+      <c r="L26" s="4">
         <v>23.5</v>
       </c>
-      <c r="M26" s="1">
+      <c r="M26" s="4">
         <v>23.7</v>
       </c>
     </row>
     <row r="27" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="4">
+      <c r="B27" s="1">
         <v>5.3000000000000203</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="4">
         <v>21.3</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="4">
         <v>21.6</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="4">
         <v>21.9</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="4">
         <v>22.2</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="4">
         <v>22.5</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="4">
         <v>22.8</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="4">
         <v>23</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27" s="4">
         <v>23.2</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="4">
         <v>23.4</v>
       </c>
-      <c r="L27" s="1">
+      <c r="L27" s="4">
         <v>23.6</v>
       </c>
-      <c r="M27" s="1">
+      <c r="M27" s="4">
         <v>23.8</v>
       </c>
     </row>
     <row r="28" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="4">
+      <c r="B28" s="1">
         <v>5.4000000000000199</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="4">
         <v>21.4</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="4">
         <v>21.7</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="4">
         <v>22</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="4">
         <v>22.3</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="4">
         <v>22.6</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="4">
         <v>22.9</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="4">
         <v>23.1</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28" s="4">
         <v>23.3</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="4">
         <v>23.5</v>
       </c>
-      <c r="L28" s="1">
+      <c r="L28" s="4">
         <v>23.7</v>
       </c>
-      <c r="M28" s="1">
+      <c r="M28" s="4">
         <v>23.9</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="4">
+      <c r="B29" s="1">
         <v>5.5000000000000204</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="4">
         <v>21.5</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="4">
         <v>21.8</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="4">
         <v>22.1</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="4">
         <v>22.4</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="4">
         <v>22.7</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="4">
         <v>23</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="4">
         <v>23.2</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="4">
         <v>23.4</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="4">
         <v>23.6</v>
       </c>
-      <c r="L29" s="1">
+      <c r="L29" s="4">
         <v>23.8</v>
       </c>
-      <c r="M29" s="1">
+      <c r="M29" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="5">
+      <c r="C32" s="2">
         <v>7</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="2">
         <v>7.1</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="2">
         <v>7.2</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="2">
         <v>7.3</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="2">
         <v>7.4</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="2">
         <v>7.5</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I32" s="2">
         <v>7.6</v>
       </c>
-      <c r="J32" s="5">
+      <c r="J32" s="2">
         <v>7.7</v>
       </c>
-      <c r="K32" s="5">
+      <c r="K32" s="2">
         <v>7.8</v>
       </c>
-      <c r="L32" s="5">
+      <c r="L32" s="2">
         <v>7.9</v>
       </c>
-      <c r="M32" s="5">
+      <c r="M32" s="2">
         <v>8</v>
       </c>
-      <c r="N32" s="5">
+      <c r="N32" s="2">
         <v>8.1</v>
       </c>
-      <c r="O32" s="5">
+      <c r="O32" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="P32" s="5">
+      <c r="P32" s="2">
         <v>8.3000000000000007</v>
       </c>
-      <c r="Q32" s="5">
+      <c r="Q32" s="2">
         <v>8.4</v>
       </c>
-      <c r="R32" s="5">
+      <c r="R32" s="2">
         <v>8.5</v>
       </c>
     </row>
     <row r="33" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="6">
+      <c r="B33" s="3">
         <v>2</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="5">
         <v>10.5</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="5">
         <v>10.8</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="5">
         <v>11.1</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="5">
         <v>11.4</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="5">
         <v>11.7</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="5">
         <v>12</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="5">
         <v>12.3</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="5">
         <v>12.6</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="5">
         <v>12.9</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="5">
         <v>13.2</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="5">
         <v>13.5</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="5">
         <v>13.8</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="5">
         <v>14.1</v>
       </c>
-      <c r="P33">
+      <c r="P33" s="5">
         <v>14.4</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="5">
         <v>14.7</v>
       </c>
-      <c r="R33">
+      <c r="R33" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="6">
+      <c r="B34" s="3">
         <v>2.1</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="5">
         <v>10.5</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="5">
         <v>10.8</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="5">
         <v>11.1</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="5">
         <v>11.4</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="5">
         <v>11.7</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="5">
         <v>12</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="5">
         <v>12.3</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="5">
         <v>12.6</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="5">
         <v>12.9</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="5">
         <v>13.2</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="5">
         <v>13.5</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="5">
         <v>13.8</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="5">
         <v>14.1</v>
       </c>
-      <c r="P34">
+      <c r="P34" s="5">
         <v>14.4</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="5">
         <v>14.7</v>
       </c>
-      <c r="R34">
+      <c r="R34" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="35" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="6">
+      <c r="B35" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="5">
         <v>10.5</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="5">
         <v>10.8</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="5">
         <v>11.1</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="5">
         <v>11.4</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="5">
         <v>11.7</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="5">
         <v>12</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="5">
         <v>12.3</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="5">
         <v>12.6</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="5">
         <v>12.9</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="5">
         <v>13.2</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="5">
         <v>13.5</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="5">
         <v>13.8</v>
       </c>
-      <c r="O35">
+      <c r="O35" s="5">
         <v>14.1</v>
       </c>
-      <c r="P35">
+      <c r="P35" s="5">
         <v>14.4</v>
       </c>
-      <c r="Q35">
+      <c r="Q35" s="5">
         <v>14.7</v>
       </c>
-      <c r="R35">
+      <c r="R35" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="6">
+      <c r="B36" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="5">
         <v>10.5</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="5">
         <v>10.8</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="5">
         <v>11.1</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="5">
         <v>11.4</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="5">
         <v>11.7</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="5">
         <v>12</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="5">
         <v>12.3</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="5">
         <v>12.6</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="5">
         <v>12.9</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="5">
         <v>13.2</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="5">
         <v>13.5</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="5">
         <v>13.8</v>
       </c>
-      <c r="O36">
+      <c r="O36" s="5">
         <v>14.1</v>
       </c>
-      <c r="P36">
+      <c r="P36" s="5">
         <v>14.4</v>
       </c>
-      <c r="Q36">
+      <c r="Q36" s="5">
         <v>14.7</v>
       </c>
-      <c r="R36">
+      <c r="R36" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="6">
+      <c r="B37" s="3">
         <v>2.4</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="5">
         <v>10.5</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="5">
         <v>10.8</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="5">
         <v>11.1</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="5">
         <v>11.4</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="5">
         <v>11.7</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="5">
         <v>12</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="5">
         <v>12.3</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="5">
         <v>12.6</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="5">
         <v>12.9</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="5">
         <v>13.2</v>
       </c>
-      <c r="M37">
+      <c r="M37" s="5">
         <v>13.5</v>
       </c>
-      <c r="N37">
+      <c r="N37" s="5">
         <v>13.8</v>
       </c>
-      <c r="O37">
+      <c r="O37" s="5">
         <v>14.1</v>
       </c>
-      <c r="P37">
+      <c r="P37" s="5">
         <v>14.4</v>
       </c>
-      <c r="Q37">
+      <c r="Q37" s="5">
         <v>14.7</v>
       </c>
-      <c r="R37">
+      <c r="R37" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="38" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="6">
+      <c r="B38" s="3">
         <v>2.5</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="5">
         <v>10.5</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="5">
         <v>10.8</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="5">
         <v>11.1</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="5">
         <v>11.4</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="5">
         <v>11.7</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="5">
         <v>12</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="5">
         <v>12.3</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="5">
         <v>12.6</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="5">
         <v>12.9</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="5">
         <v>13.2</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="5">
         <v>13.5</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="5">
         <v>13.8</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="5">
         <v>14.1</v>
       </c>
-      <c r="P38">
+      <c r="P38" s="5">
         <v>14.4</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="5">
         <v>14.7</v>
       </c>
-      <c r="R38">
+      <c r="R38" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="39" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="6">
+      <c r="B39" s="3">
         <v>2.6</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="5">
         <v>11</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="5">
         <v>11.3</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="5">
         <v>11.6</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="5">
         <v>11.9</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="5">
         <v>12.2</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="5">
         <v>12.5</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="5">
         <v>12.8</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="5">
         <v>13.1</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="5">
         <v>13.4</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="5">
         <v>13.7</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="5">
         <v>14</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="5">
         <v>14.3</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="5">
         <v>14.6</v>
       </c>
-      <c r="P39">
+      <c r="P39" s="5">
         <v>14.9</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="5">
         <v>15.2</v>
       </c>
-      <c r="R39">
+      <c r="R39" s="5">
         <v>15.5</v>
       </c>
     </row>
     <row r="40" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="6">
+      <c r="B40" s="3">
         <v>2.7</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="5">
         <v>11.5</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="5">
         <v>11.8</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="5">
         <v>12.1</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="5">
         <v>12.4</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="5">
         <v>12.7</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="5">
         <v>13</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="5">
         <v>13.3</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="5">
         <v>13.6</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="5">
         <v>13.9</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="5">
         <v>14.2</v>
       </c>
-      <c r="M40">
+      <c r="M40" s="5">
         <v>14.5</v>
       </c>
-      <c r="N40">
+      <c r="N40" s="5">
         <v>14.8</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="5">
         <v>15.1</v>
       </c>
-      <c r="P40">
+      <c r="P40" s="5">
         <v>15.4</v>
       </c>
-      <c r="Q40">
+      <c r="Q40" s="5">
         <v>15.7</v>
       </c>
-      <c r="R40">
+      <c r="R40" s="5">
         <v>16</v>
       </c>
     </row>
     <row r="41" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="6">
+      <c r="B41" s="3">
         <v>2.8</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="5">
         <v>12</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="5">
         <v>12.3</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="5">
         <v>12.6</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="5">
         <v>12.9</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="5">
         <v>13.2</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="5">
         <v>13.5</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="5">
         <v>13.8</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="5">
         <v>14.1</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="5">
         <v>14.4</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="5">
         <v>14.7</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="5">
         <v>15</v>
       </c>
+      <c r="N41" s="5">
+        <v>15.3</v>
+      </c>
+      <c r="O41" s="5">
+        <v>15.6</v>
+      </c>
+      <c r="P41" s="5">
+        <v>15.9</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>16.2</v>
+      </c>
+      <c r="R41" s="5">
+        <v>16.5</v>
+      </c>
     </row>
     <row r="42" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="6">
+      <c r="B42" s="3">
         <v>2.9</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="5">
         <v>12.5</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="5">
         <v>12.8</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="5">
         <v>13.1</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="5">
         <v>13.4</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="5">
         <v>13.7</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="5">
         <v>14</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="5">
         <v>14.3</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="5">
         <v>14.6</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="5">
         <v>14.9</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="5">
         <v>15.2</v>
       </c>
-      <c r="M42">
+      <c r="M42" s="5">
         <v>15.5</v>
       </c>
-      <c r="N42">
+      <c r="N42" s="5">
         <v>15.8</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="5">
         <v>16.100000000000001</v>
       </c>
-      <c r="P42">
+      <c r="P42" s="5">
         <v>16.399999999999999</v>
       </c>
-      <c r="Q42">
+      <c r="Q42" s="5">
         <v>16.7</v>
       </c>
-      <c r="R42">
+      <c r="R42" s="5">
         <v>17</v>
       </c>
     </row>
     <row r="43" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="6">
+      <c r="B43" s="3">
         <v>3</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="5">
         <v>13</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="5">
         <v>13.3</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="5">
         <v>13.6</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="5">
         <v>13.9</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="5">
         <v>14.2</v>
       </c>
-      <c r="H43" s="3"/>
+      <c r="H43" s="4">
+        <v>18</v>
+      </c>
+      <c r="I43" s="4">
+        <v>18.3</v>
+      </c>
+      <c r="J43" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="K43" s="4">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="L43" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="M43" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="N43" s="4">
+        <v>19.7</v>
+      </c>
+      <c r="O43" s="4">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="P43" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="Q43" s="4">
+        <v>20.3</v>
+      </c>
+      <c r="R43" s="4">
+        <v>20.5</v>
+      </c>
     </row>
     <row r="44" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="6">
+      <c r="B44" s="3">
         <v>3.1</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="5">
         <v>13.5</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="5">
         <v>13.8</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="5">
         <v>14.1</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="5">
         <v>14.4</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="5">
         <v>14.7</v>
       </c>
+      <c r="H44" s="4">
+        <v>18.3</v>
+      </c>
+      <c r="I44" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="J44" s="4">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="K44" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="L44" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="M44" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="N44" s="4">
+        <v>20</v>
+      </c>
+      <c r="O44" s="4">
+        <v>20.2</v>
+      </c>
+      <c r="P44" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="R44" s="4">
+        <v>20.8</v>
+      </c>
     </row>
     <row r="45" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="6">
+      <c r="B45" s="3">
         <v>3.2</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="5">
         <v>14</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="5">
         <v>14.3</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="5">
         <v>14.6</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="5">
         <v>14.9</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="5">
         <v>15.2</v>
       </c>
+      <c r="H45" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="I45" s="4">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J45" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="K45" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="L45" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="M45" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="N45" s="4">
+        <v>20.3</v>
+      </c>
+      <c r="O45" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="P45" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="Q45" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="R45" s="4">
+        <v>21.1</v>
+      </c>
     </row>
     <row r="46" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="6">
+      <c r="B46" s="3">
         <v>3.3</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="5">
         <v>14.5</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="5">
         <v>14.8</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="5">
         <v>15.1</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="5">
         <v>15.4</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="5">
         <v>15.7</v>
       </c>
+      <c r="H46" s="4">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="I46" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="J46" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="K46" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="L46" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="M46" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="N46" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="O46" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="P46" s="4">
+        <v>21</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="R46" s="4">
+        <v>21.4</v>
+      </c>
     </row>
     <row r="47" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="6">
+      <c r="B47" s="3">
         <v>3.4</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="5">
         <v>15</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="5">
         <v>15.3</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="5">
         <v>15.6</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="5">
         <v>15.9</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="5">
         <v>16.2</v>
       </c>
+      <c r="H47" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="I47" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="J47" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="K47" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L47" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="M47" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="N47" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="O47" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="P47" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="R47" s="4">
+        <v>21.7</v>
+      </c>
     </row>
     <row r="48" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="6">
+      <c r="B48" s="3">
         <v>3.5</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="5">
         <v>15.5</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="5">
         <v>15.8</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="5">
         <v>16.100000000000001</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="5">
         <v>16.399999999999999</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="5">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="6">
+      <c r="H48" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="I48" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="J48" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="K48" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="L48" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="M48" s="4">
+        <v>21</v>
+      </c>
+      <c r="N48" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="O48" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="P48" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="R48" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="3">
         <v>3.6</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="6">
         <v>15.7</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="5">
         <v>16</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="5">
         <v>16.3</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="5">
         <v>16.600000000000001</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="5">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="6">
+      <c r="H49" s="4">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="I49" s="4">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="J49" s="4">
+        <v>20.2</v>
+      </c>
+      <c r="K49" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="L49" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="M49" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="N49" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="O49" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="P49" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="R49" s="4">
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="3">
         <v>3.7</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="5">
         <v>15.9</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="5">
         <v>16.2</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="5">
         <v>16.5</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50" s="5">
         <v>16.8</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="5">
         <v>17.100000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="6">
+      <c r="H50" s="4">
+        <v>19.7</v>
+      </c>
+      <c r="I50" s="4">
+        <v>20</v>
+      </c>
+      <c r="J50" s="4">
+        <v>20.3</v>
+      </c>
+      <c r="K50" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="L50" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="M50" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="N50" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="O50" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="P50" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>22</v>
+      </c>
+      <c r="R50" s="4">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="3">
         <v>3.8</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="5">
         <v>16.100000000000001</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="5">
         <v>16.399999999999999</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="5">
         <v>16.7</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51" s="5">
         <v>17</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="5">
         <v>17.3</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="6">
+      <c r="H51" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="I51" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J51" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K51" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="L51" s="4">
+        <v>21</v>
+      </c>
+      <c r="M51" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="N51" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="O51" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="P51" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="R51" s="4">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="3">
         <v>3.9</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="5">
         <v>16.3</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="5">
         <v>16.600000000000001</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="5">
         <v>16.899999999999999</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52" s="5">
         <v>17.2</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52" s="5">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="6">
+      <c r="H52" s="4">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="I52" s="4">
+        <v>20.2</v>
+      </c>
+      <c r="J52" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="K52" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="L52" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="M52" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="N52" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="O52" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="P52" s="4">
+        <v>22</v>
+      </c>
+      <c r="Q52" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="R52" s="4">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="3">
         <v>4</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="5">
         <v>16.5</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="5">
         <v>16.8</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="5">
         <v>17.100000000000001</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53" s="5">
         <v>17.399999999999999</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53" s="5">
         <v>17.7</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="6">
+      <c r="H53" s="4">
+        <v>20</v>
+      </c>
+      <c r="I53" s="4">
+        <v>20.3</v>
+      </c>
+      <c r="J53" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="K53" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="L53" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="M53" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="N53" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="O53" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="P53" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="R53" s="4">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="5">
         <v>16.7</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="5">
         <v>17</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="5">
         <v>17.3</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54" s="5">
         <v>17.600000000000001</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="5">
         <v>17.899999999999999</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="6">
+      <c r="H54" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I54" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J54" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="K54" s="4">
+        <v>21</v>
+      </c>
+      <c r="L54" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="M54" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="N54" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="O54" s="4">
+        <v>22</v>
+      </c>
+      <c r="P54" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="R54" s="4">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="3">
         <v>4.2</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="5">
         <v>16.899999999999999</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="5">
         <v>17.2</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="5">
         <v>17.5</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F55" s="5">
         <v>17.8</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="5">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="6">
+      <c r="H55" s="4">
+        <v>20.2</v>
+      </c>
+      <c r="I55" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="J55" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="K55" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="L55" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="M55" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="N55" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="O55" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="P55" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="R55" s="4">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="56" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="3">
         <v>4.3</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="5">
         <v>17.100000000000001</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="5">
         <v>17.399999999999999</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="5">
         <v>17.7</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F56" s="5">
         <v>18</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G56" s="5">
         <v>18.3</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="6">
+      <c r="H56" s="4">
+        <v>20.3</v>
+      </c>
+      <c r="I56" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="J56" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="K56" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="L56" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="M56" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="N56" s="4">
+        <v>22</v>
+      </c>
+      <c r="O56" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="P56" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="Q56" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="R56" s="4">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="5">
         <v>17.3</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="5">
         <v>17.600000000000001</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="5">
         <v>17.899999999999999</v>
       </c>
-      <c r="F57" s="3">
+      <c r="F57" s="5">
         <v>18.2</v>
       </c>
-      <c r="G57" s="3">
+      <c r="G57" s="5">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="58" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="6">
+      <c r="H57" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="I57" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="J57" s="4">
+        <v>21</v>
+      </c>
+      <c r="K57" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="L57" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="M57" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="N57" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="O57" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="P57" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="Q57" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="R57" s="4">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="3">
         <v>4.5</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="5">
         <v>17.5</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="5">
         <v>17.8</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="5">
         <v>18.100000000000001</v>
       </c>
-      <c r="F58" s="3">
+      <c r="F58" s="5">
         <v>18.399999999999999</v>
       </c>
-      <c r="G58" s="3">
+      <c r="G58" s="5">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="59" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="6">
+      <c r="H58" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="I58" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="J58" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="K58" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="L58" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="M58" s="4">
+        <v>22</v>
+      </c>
+      <c r="N58" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="O58" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="P58" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="Q58" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="R58" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="5">
         <v>17.7</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="5">
         <v>18</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="5">
         <v>18.3</v>
       </c>
-      <c r="F59" s="3">
+      <c r="F59" s="5">
         <v>18.600000000000001</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G59" s="5">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="6">
+      <c r="H59" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="I59" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="J59" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="K59" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="L59" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="M59" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="N59" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="O59" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="P59" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="Q59" s="4">
+        <v>22.9</v>
+      </c>
+      <c r="R59" s="4">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="3">
         <v>4.7</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="5">
         <v>17.899999999999999</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="5">
         <v>18.2</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="5">
         <v>18.5</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F60" s="5">
         <v>18.8</v>
       </c>
-      <c r="G60" s="3">
+      <c r="G60" s="5">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="6">
+      <c r="H60" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="I60" s="4">
+        <v>21</v>
+      </c>
+      <c r="J60" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="K60" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="L60" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="M60" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="N60" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="O60" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="P60" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="Q60" s="4">
+        <v>23</v>
+      </c>
+      <c r="R60" s="4">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="3">
         <v>4.8</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="5">
         <v>18.100000000000001</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="5">
         <v>18.399999999999999</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61" s="5">
         <v>18.7</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61" s="5">
         <v>19</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G61" s="5">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="6">
+      <c r="H61" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="I61" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="J61" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="K61" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="L61" s="4">
+        <v>22</v>
+      </c>
+      <c r="M61" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="N61" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="O61" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="P61" s="4">
+        <v>22.9</v>
+      </c>
+      <c r="Q61" s="4">
+        <v>23.1</v>
+      </c>
+      <c r="R61" s="4">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="5">
         <v>18.3</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="5">
         <v>18.600000000000001</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E62" s="5">
         <v>18.899999999999999</v>
       </c>
-      <c r="F62" s="3">
+      <c r="F62" s="5">
         <v>19.2</v>
       </c>
-      <c r="G62" s="3">
+      <c r="G62" s="5">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="63" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="6">
+      <c r="H62" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="I62" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="J62" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="K62" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="L62" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="M62" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="N62" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="O62" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="P62" s="4">
+        <v>23</v>
+      </c>
+      <c r="Q62" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="R62" s="4">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="3">
         <v>5</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="5">
         <v>18.5</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="5">
         <v>18.8</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E63" s="5">
         <v>19.100000000000001</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F63" s="5">
         <v>19.399999999999999</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G63" s="5">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="64" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="6">
+      <c r="H63" s="4">
+        <v>21</v>
+      </c>
+      <c r="I63" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="J63" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="K63" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="L63" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="M63" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="N63" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="O63" s="4">
+        <v>22.9</v>
+      </c>
+      <c r="P63" s="4">
+        <v>23.1</v>
+      </c>
+      <c r="Q63" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="R63" s="4">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="64" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="5">
         <v>18.7</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="5">
         <v>19</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E64" s="5">
         <v>19.3</v>
       </c>
-      <c r="F64" s="3">
+      <c r="F64" s="5">
         <v>19.600000000000001</v>
       </c>
-      <c r="G64" s="3">
+      <c r="G64" s="5">
         <v>19.899999999999999</v>
       </c>
-    </row>
-    <row r="65" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="6">
+      <c r="H64" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="I64" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="J64" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="K64" s="4">
+        <v>22</v>
+      </c>
+      <c r="L64" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="M64" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="N64" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="O64" s="4">
+        <v>23</v>
+      </c>
+      <c r="P64" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="Q64" s="4">
+        <v>23.4</v>
+      </c>
+      <c r="R64" s="4">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="3">
         <v>5.2</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="5">
         <v>18.899999999999999</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="5">
         <v>19.2</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E65" s="5">
         <v>19.5</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F65" s="5">
         <v>19.8</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G65" s="5">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="66" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="6">
+      <c r="H65" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="I65" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="J65" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="K65" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="L65" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="M65" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="N65" s="4">
+        <v>22.9</v>
+      </c>
+      <c r="O65" s="4">
+        <v>23.1</v>
+      </c>
+      <c r="P65" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="Q65" s="4">
+        <v>23.5</v>
+      </c>
+      <c r="R65" s="4">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="3">
         <v>5.3</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C66" s="5">
         <v>19.100000000000001</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="5">
         <v>19.399999999999999</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66" s="5">
         <v>19.7</v>
       </c>
-      <c r="F66" s="3">
+      <c r="F66" s="5">
         <v>20</v>
       </c>
-      <c r="G66" s="3">
+      <c r="G66" s="5">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="67" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="6">
+      <c r="H66" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="I66" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="J66" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="K66" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="L66" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="M66" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="N66" s="4">
+        <v>23</v>
+      </c>
+      <c r="O66" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="P66" s="4">
+        <v>23.4</v>
+      </c>
+      <c r="Q66" s="4">
+        <v>23.6</v>
+      </c>
+      <c r="R66" s="4">
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="3">
         <v>5.4</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="5">
         <v>19.3</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="5">
         <v>19.600000000000001</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E67" s="5">
         <v>19.899999999999999</v>
       </c>
-      <c r="F67" s="3">
+      <c r="F67" s="5">
         <v>20.2</v>
       </c>
-      <c r="G67" s="3">
+      <c r="G67" s="5">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="68" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="6">
+      <c r="H67" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="I67" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="J67" s="4">
+        <v>22</v>
+      </c>
+      <c r="K67" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="L67" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="M67" s="4">
+        <v>22.9</v>
+      </c>
+      <c r="N67" s="4">
+        <v>23.1</v>
+      </c>
+      <c r="O67" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="P67" s="4">
+        <v>23.5</v>
+      </c>
+      <c r="Q67" s="4">
+        <v>23.7</v>
+      </c>
+      <c r="R67" s="4">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="68" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="3">
         <v>5.5</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="5">
         <v>19.5</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="5">
         <v>19.8</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E68" s="5">
         <v>20.100000000000001</v>
       </c>
-      <c r="F68" s="3">
+      <c r="F68" s="5">
         <v>20.399999999999999</v>
       </c>
-      <c r="G68" s="3">
+      <c r="G68" s="5">
         <v>20.7</v>
       </c>
+      <c r="H68" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="I68" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="J68" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="K68" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="L68" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="M68" s="4">
+        <v>23</v>
+      </c>
+      <c r="N68" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="O68" s="4">
+        <v>23.4</v>
+      </c>
+      <c r="P68" s="4">
+        <v>23.6</v>
+      </c>
+      <c r="Q68" s="4">
+        <v>23.8</v>
+      </c>
+      <c r="R68" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Laxman : Added LPGlobalVariables class
</commit_message>
<xml_diff>
--- a/Milk_Rate_Chart_Template.xlsx
+++ b/Milk_Rate_Chart_Template.xlsx
@@ -314,8 +314,8 @@
   </sheetPr>
   <dimension ref="B3:R69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1942,38 +1942,38 @@
       <c r="G43" s="5">
         <v>14.2</v>
       </c>
-      <c r="H43" s="4">
-        <v>18</v>
-      </c>
-      <c r="I43" s="4">
-        <v>18.3</v>
-      </c>
-      <c r="J43" s="4">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="K43" s="4">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="L43" s="4">
-        <v>19.2</v>
-      </c>
-      <c r="M43" s="4">
-        <v>19.5</v>
-      </c>
-      <c r="N43" s="4">
-        <v>19.7</v>
-      </c>
-      <c r="O43" s="4">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="P43" s="4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="Q43" s="4">
-        <v>20.3</v>
-      </c>
-      <c r="R43" s="4">
-        <v>20.5</v>
+      <c r="H43" s="5">
+        <v>14.5</v>
+      </c>
+      <c r="I43" s="5">
+        <v>14.8</v>
+      </c>
+      <c r="J43" s="5">
+        <v>15.1</v>
+      </c>
+      <c r="K43" s="5">
+        <v>15.4</v>
+      </c>
+      <c r="L43" s="5">
+        <v>15.7</v>
+      </c>
+      <c r="M43" s="5">
+        <v>16</v>
+      </c>
+      <c r="N43" s="5">
+        <v>16.3</v>
+      </c>
+      <c r="O43" s="5">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="P43" s="5">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>17.2</v>
+      </c>
+      <c r="R43" s="5">
+        <v>17.5</v>
       </c>
     </row>
     <row r="44" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1995,38 +1995,38 @@
       <c r="G44" s="5">
         <v>14.7</v>
       </c>
-      <c r="H44" s="4">
-        <v>18.3</v>
-      </c>
-      <c r="I44" s="4">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="J44" s="4">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="K44" s="4">
-        <v>19.2</v>
-      </c>
-      <c r="L44" s="4">
-        <v>19.5</v>
-      </c>
-      <c r="M44" s="4">
-        <v>19.8</v>
-      </c>
-      <c r="N44" s="4">
-        <v>20</v>
-      </c>
-      <c r="O44" s="4">
-        <v>20.2</v>
-      </c>
-      <c r="P44" s="4">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="Q44" s="4">
-        <v>20.6</v>
-      </c>
-      <c r="R44" s="4">
-        <v>20.8</v>
+      <c r="H44" s="5">
+        <v>15</v>
+      </c>
+      <c r="I44" s="5">
+        <v>15.3</v>
+      </c>
+      <c r="J44" s="5">
+        <v>15.6</v>
+      </c>
+      <c r="K44" s="5">
+        <v>15.9</v>
+      </c>
+      <c r="L44" s="5">
+        <v>16.2</v>
+      </c>
+      <c r="M44" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="N44" s="5">
+        <v>16.8</v>
+      </c>
+      <c r="O44" s="5">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="P44" s="5">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>17.7</v>
+      </c>
+      <c r="R44" s="5">
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2048,38 +2048,38 @@
       <c r="G45" s="5">
         <v>15.2</v>
       </c>
-      <c r="H45" s="4">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="I45" s="4">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="J45" s="4">
-        <v>19.2</v>
-      </c>
-      <c r="K45" s="4">
-        <v>19.5</v>
-      </c>
-      <c r="L45" s="4">
-        <v>19.8</v>
-      </c>
-      <c r="M45" s="4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="N45" s="4">
-        <v>20.3</v>
-      </c>
-      <c r="O45" s="4">
-        <v>20.5</v>
-      </c>
-      <c r="P45" s="4">
-        <v>20.7</v>
-      </c>
-      <c r="Q45" s="4">
-        <v>20.9</v>
-      </c>
-      <c r="R45" s="4">
-        <v>21.1</v>
+      <c r="H45" s="5">
+        <v>15.5</v>
+      </c>
+      <c r="I45" s="5">
+        <v>15.8</v>
+      </c>
+      <c r="J45" s="5">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="K45" s="5">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="L45" s="5">
+        <v>16.7</v>
+      </c>
+      <c r="M45" s="5">
+        <v>17</v>
+      </c>
+      <c r="N45" s="5">
+        <v>17.3</v>
+      </c>
+      <c r="O45" s="5">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="P45" s="5">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="Q45" s="5">
+        <v>18.2</v>
+      </c>
+      <c r="R45" s="5">
+        <v>18.5</v>
       </c>
     </row>
     <row r="46" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2101,38 +2101,38 @@
       <c r="G46" s="5">
         <v>15.7</v>
       </c>
-      <c r="H46" s="4">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="I46" s="4">
-        <v>19.2</v>
-      </c>
-      <c r="J46" s="4">
-        <v>19.5</v>
-      </c>
-      <c r="K46" s="4">
-        <v>19.8</v>
-      </c>
-      <c r="L46" s="4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="M46" s="4">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="N46" s="4">
-        <v>20.6</v>
-      </c>
-      <c r="O46" s="4">
-        <v>20.8</v>
-      </c>
-      <c r="P46" s="4">
-        <v>21</v>
-      </c>
-      <c r="Q46" s="4">
-        <v>21.2</v>
-      </c>
-      <c r="R46" s="4">
-        <v>21.4</v>
+      <c r="H46" s="5">
+        <v>16</v>
+      </c>
+      <c r="I46" s="5">
+        <v>16.3</v>
+      </c>
+      <c r="J46" s="5">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="K46" s="5">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="L46" s="5">
+        <v>17.2</v>
+      </c>
+      <c r="M46" s="5">
+        <v>17.5</v>
+      </c>
+      <c r="N46" s="5">
+        <v>17.8</v>
+      </c>
+      <c r="O46" s="5">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="P46" s="5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="Q46" s="5">
+        <v>18.7</v>
+      </c>
+      <c r="R46" s="5">
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2154,38 +2154,38 @@
       <c r="G47" s="5">
         <v>16.2</v>
       </c>
-      <c r="H47" s="4">
+      <c r="H47" s="5">
+        <v>16.5</v>
+      </c>
+      <c r="I47" s="5">
+        <v>16.8</v>
+      </c>
+      <c r="J47" s="5">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="K47" s="5">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="L47" s="5">
+        <v>17.7</v>
+      </c>
+      <c r="M47" s="5">
+        <v>18</v>
+      </c>
+      <c r="N47" s="5">
+        <v>18.3</v>
+      </c>
+      <c r="O47" s="5">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="P47" s="5">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="Q47" s="5">
         <v>19.2</v>
       </c>
-      <c r="I47" s="4">
+      <c r="R47" s="5">
         <v>19.5</v>
-      </c>
-      <c r="J47" s="4">
-        <v>19.8</v>
-      </c>
-      <c r="K47" s="4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L47" s="4">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="M47" s="4">
-        <v>20.7</v>
-      </c>
-      <c r="N47" s="4">
-        <v>20.9</v>
-      </c>
-      <c r="O47" s="4">
-        <v>21.1</v>
-      </c>
-      <c r="P47" s="4">
-        <v>21.3</v>
-      </c>
-      <c r="Q47" s="4">
-        <v>21.5</v>
-      </c>
-      <c r="R47" s="4">
-        <v>21.7</v>
       </c>
     </row>
     <row r="48" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2207,38 +2207,38 @@
       <c r="G48" s="5">
         <v>16.7</v>
       </c>
-      <c r="H48" s="4">
-        <v>19.5</v>
-      </c>
-      <c r="I48" s="4">
-        <v>19.8</v>
-      </c>
-      <c r="J48" s="4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="K48" s="4">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="L48" s="4">
-        <v>20.7</v>
-      </c>
-      <c r="M48" s="4">
-        <v>21</v>
-      </c>
-      <c r="N48" s="4">
-        <v>21.2</v>
-      </c>
-      <c r="O48" s="4">
-        <v>21.4</v>
-      </c>
-      <c r="P48" s="4">
-        <v>21.6</v>
-      </c>
-      <c r="Q48" s="4">
-        <v>21.8</v>
-      </c>
-      <c r="R48" s="4">
-        <v>22</v>
+      <c r="H48" s="5">
+        <v>17</v>
+      </c>
+      <c r="I48" s="5">
+        <v>17.3</v>
+      </c>
+      <c r="J48" s="5">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="K48" s="5">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="L48" s="5">
+        <v>18.2</v>
+      </c>
+      <c r="M48" s="5">
+        <v>18.5</v>
+      </c>
+      <c r="N48" s="5">
+        <v>18.8</v>
+      </c>
+      <c r="O48" s="5">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="P48" s="5">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="Q48" s="5">
+        <v>19.7</v>
+      </c>
+      <c r="R48" s="5">
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2260,38 +2260,38 @@
       <c r="G49" s="5">
         <v>16.899999999999999</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H49" s="6">
+        <v>17.2</v>
+      </c>
+      <c r="I49" s="5">
+        <v>17.5</v>
+      </c>
+      <c r="J49" s="5">
+        <v>17.8</v>
+      </c>
+      <c r="K49" s="5">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="L49" s="5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="M49" s="6">
+        <v>18.7</v>
+      </c>
+      <c r="N49" s="5">
+        <v>19</v>
+      </c>
+      <c r="O49" s="5">
+        <v>19.3</v>
+      </c>
+      <c r="P49" s="5">
         <v>19.600000000000001</v>
       </c>
-      <c r="I49" s="4">
+      <c r="Q49" s="5">
         <v>19.899999999999999</v>
       </c>
-      <c r="J49" s="4">
+      <c r="R49" s="6">
         <v>20.2</v>
-      </c>
-      <c r="K49" s="4">
-        <v>20.5</v>
-      </c>
-      <c r="L49" s="4">
-        <v>20.8</v>
-      </c>
-      <c r="M49" s="4">
-        <v>21.1</v>
-      </c>
-      <c r="N49" s="4">
-        <v>21.3</v>
-      </c>
-      <c r="O49" s="4">
-        <v>21.5</v>
-      </c>
-      <c r="P49" s="4">
-        <v>21.7</v>
-      </c>
-      <c r="Q49" s="4">
-        <v>21.9</v>
-      </c>
-      <c r="R49" s="4">
-        <v>22.1</v>
       </c>
     </row>
     <row r="50" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2313,38 +2313,38 @@
       <c r="G50" s="5">
         <v>17.100000000000001</v>
       </c>
-      <c r="H50" s="4">
-        <v>19.7</v>
-      </c>
-      <c r="I50" s="4">
-        <v>20</v>
-      </c>
-      <c r="J50" s="4">
-        <v>20.3</v>
-      </c>
-      <c r="K50" s="4">
-        <v>20.6</v>
-      </c>
-      <c r="L50" s="4">
-        <v>20.9</v>
-      </c>
-      <c r="M50" s="4">
-        <v>21.2</v>
-      </c>
-      <c r="N50" s="4">
-        <v>21.4</v>
-      </c>
-      <c r="O50" s="4">
-        <v>21.6</v>
-      </c>
-      <c r="P50" s="4">
-        <v>21.8</v>
-      </c>
-      <c r="Q50" s="4">
-        <v>22</v>
-      </c>
-      <c r="R50" s="4">
-        <v>22.2</v>
+      <c r="H50" s="5">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="I50" s="5">
+        <v>17.7</v>
+      </c>
+      <c r="J50" s="5">
+        <v>18</v>
+      </c>
+      <c r="K50" s="5">
+        <v>18.3</v>
+      </c>
+      <c r="L50" s="5">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="M50" s="5">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="N50" s="5">
+        <v>19.2</v>
+      </c>
+      <c r="O50" s="5">
+        <v>19.5</v>
+      </c>
+      <c r="P50" s="5">
+        <v>19.8</v>
+      </c>
+      <c r="Q50" s="5">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="R50" s="5">
+        <v>20.399999999999999</v>
       </c>
     </row>
     <row r="51" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2366,38 +2366,38 @@
       <c r="G51" s="5">
         <v>17.3</v>
       </c>
-      <c r="H51" s="4">
-        <v>19.8</v>
-      </c>
-      <c r="I51" s="4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="J51" s="4">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="K51" s="4">
-        <v>20.7</v>
-      </c>
-      <c r="L51" s="4">
-        <v>21</v>
-      </c>
-      <c r="M51" s="4">
-        <v>21.3</v>
-      </c>
-      <c r="N51" s="4">
-        <v>21.5</v>
-      </c>
-      <c r="O51" s="4">
-        <v>21.7</v>
-      </c>
-      <c r="P51" s="4">
-        <v>21.9</v>
-      </c>
-      <c r="Q51" s="4">
-        <v>22.1</v>
-      </c>
-      <c r="R51" s="4">
-        <v>22.3</v>
+      <c r="H51" s="5">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="I51" s="5">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="J51" s="5">
+        <v>18.2</v>
+      </c>
+      <c r="K51" s="5">
+        <v>18.5</v>
+      </c>
+      <c r="L51" s="5">
+        <v>18.8</v>
+      </c>
+      <c r="M51" s="5">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="N51" s="5">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="O51" s="5">
+        <v>19.7</v>
+      </c>
+      <c r="P51" s="5">
+        <v>20</v>
+      </c>
+      <c r="Q51" s="5">
+        <v>20.3</v>
+      </c>
+      <c r="R51" s="5">
+        <v>20.6</v>
       </c>
     </row>
     <row r="52" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2419,38 +2419,38 @@
       <c r="G52" s="5">
         <v>17.5</v>
       </c>
-      <c r="H52" s="4">
+      <c r="H52" s="5">
+        <v>17.8</v>
+      </c>
+      <c r="I52" s="5">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="J52" s="5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="K52" s="5">
+        <v>18.7</v>
+      </c>
+      <c r="L52" s="5">
+        <v>19</v>
+      </c>
+      <c r="M52" s="5">
+        <v>19.3</v>
+      </c>
+      <c r="N52" s="5">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="O52" s="5">
         <v>19.899999999999999</v>
       </c>
-      <c r="I52" s="4">
+      <c r="P52" s="5">
         <v>20.2</v>
       </c>
-      <c r="J52" s="4">
+      <c r="Q52" s="5">
         <v>20.5</v>
       </c>
-      <c r="K52" s="4">
+      <c r="R52" s="5">
         <v>20.8</v>
-      </c>
-      <c r="L52" s="4">
-        <v>21.1</v>
-      </c>
-      <c r="M52" s="4">
-        <v>21.4</v>
-      </c>
-      <c r="N52" s="4">
-        <v>21.6</v>
-      </c>
-      <c r="O52" s="4">
-        <v>21.8</v>
-      </c>
-      <c r="P52" s="4">
-        <v>22</v>
-      </c>
-      <c r="Q52" s="4">
-        <v>22.2</v>
-      </c>
-      <c r="R52" s="4">
-        <v>22.4</v>
       </c>
     </row>
     <row r="53" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2472,38 +2472,38 @@
       <c r="G53" s="5">
         <v>17.7</v>
       </c>
-      <c r="H53" s="4">
-        <v>20</v>
-      </c>
-      <c r="I53" s="4">
-        <v>20.3</v>
-      </c>
-      <c r="J53" s="4">
-        <v>20.6</v>
-      </c>
-      <c r="K53" s="4">
-        <v>20.9</v>
-      </c>
-      <c r="L53" s="4">
-        <v>21.2</v>
-      </c>
-      <c r="M53" s="4">
-        <v>21.5</v>
-      </c>
-      <c r="N53" s="4">
-        <v>21.7</v>
-      </c>
-      <c r="O53" s="4">
-        <v>21.9</v>
-      </c>
-      <c r="P53" s="4">
-        <v>22.1</v>
-      </c>
-      <c r="Q53" s="4">
-        <v>22.3</v>
-      </c>
-      <c r="R53" s="4">
-        <v>22.5</v>
+      <c r="H53" s="5">
+        <v>18</v>
+      </c>
+      <c r="I53" s="5">
+        <v>18.3</v>
+      </c>
+      <c r="J53" s="5">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="K53" s="5">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="L53" s="5">
+        <v>19.2</v>
+      </c>
+      <c r="M53" s="5">
+        <v>19.5</v>
+      </c>
+      <c r="N53" s="5">
+        <v>19.8</v>
+      </c>
+      <c r="O53" s="5">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="P53" s="5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="Q53" s="5">
+        <v>20.7</v>
+      </c>
+      <c r="R53" s="5">
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2525,38 +2525,38 @@
       <c r="G54" s="5">
         <v>17.899999999999999</v>
       </c>
-      <c r="H54" s="4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="I54" s="4">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="J54" s="4">
-        <v>20.7</v>
-      </c>
-      <c r="K54" s="4">
-        <v>21</v>
-      </c>
-      <c r="L54" s="4">
-        <v>21.3</v>
-      </c>
-      <c r="M54" s="4">
-        <v>21.6</v>
-      </c>
-      <c r="N54" s="4">
-        <v>21.8</v>
-      </c>
-      <c r="O54" s="4">
-        <v>22</v>
-      </c>
-      <c r="P54" s="4">
-        <v>22.2</v>
-      </c>
-      <c r="Q54" s="4">
-        <v>22.4</v>
-      </c>
-      <c r="R54" s="4">
-        <v>22.6</v>
+      <c r="H54" s="5">
+        <v>18.2</v>
+      </c>
+      <c r="I54" s="5">
+        <v>18.5</v>
+      </c>
+      <c r="J54" s="5">
+        <v>18.8</v>
+      </c>
+      <c r="K54" s="5">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="L54" s="5">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="M54" s="5">
+        <v>19.7</v>
+      </c>
+      <c r="N54" s="5">
+        <v>20</v>
+      </c>
+      <c r="O54" s="5">
+        <v>20.3</v>
+      </c>
+      <c r="P54" s="5">
+        <v>20.6</v>
+      </c>
+      <c r="Q54" s="5">
+        <v>20.9</v>
+      </c>
+      <c r="R54" s="5">
+        <v>21.2</v>
       </c>
     </row>
     <row r="55" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2578,38 +2578,38 @@
       <c r="G55" s="5">
         <v>18.100000000000001</v>
       </c>
-      <c r="H55" s="4">
+      <c r="H55" s="5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="I55" s="5">
+        <v>18.7</v>
+      </c>
+      <c r="J55" s="5">
+        <v>19</v>
+      </c>
+      <c r="K55" s="5">
+        <v>19.3</v>
+      </c>
+      <c r="L55" s="5">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="M55" s="5">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="N55" s="5">
         <v>20.2</v>
       </c>
-      <c r="I55" s="4">
+      <c r="O55" s="5">
         <v>20.5</v>
       </c>
-      <c r="J55" s="4">
+      <c r="P55" s="5">
         <v>20.8</v>
       </c>
-      <c r="K55" s="4">
+      <c r="Q55" s="5">
         <v>21.1</v>
       </c>
-      <c r="L55" s="4">
+      <c r="R55" s="5">
         <v>21.4</v>
-      </c>
-      <c r="M55" s="4">
-        <v>21.7</v>
-      </c>
-      <c r="N55" s="4">
-        <v>21.9</v>
-      </c>
-      <c r="O55" s="4">
-        <v>22.1</v>
-      </c>
-      <c r="P55" s="4">
-        <v>22.3</v>
-      </c>
-      <c r="Q55" s="4">
-        <v>22.5</v>
-      </c>
-      <c r="R55" s="4">
-        <v>22.7</v>
       </c>
     </row>
     <row r="56" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2631,38 +2631,38 @@
       <c r="G56" s="5">
         <v>18.3</v>
       </c>
-      <c r="H56" s="4">
-        <v>20.3</v>
-      </c>
-      <c r="I56" s="4">
-        <v>20.6</v>
-      </c>
-      <c r="J56" s="4">
-        <v>20.9</v>
-      </c>
-      <c r="K56" s="4">
-        <v>21.2</v>
-      </c>
-      <c r="L56" s="4">
-        <v>21.5</v>
-      </c>
-      <c r="M56" s="4">
-        <v>21.8</v>
-      </c>
-      <c r="N56" s="4">
-        <v>22</v>
-      </c>
-      <c r="O56" s="4">
-        <v>22.2</v>
-      </c>
-      <c r="P56" s="4">
-        <v>22.4</v>
-      </c>
-      <c r="Q56" s="4">
-        <v>22.6</v>
-      </c>
-      <c r="R56" s="4">
-        <v>22.8</v>
+      <c r="H56" s="5">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="I56" s="5">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J56" s="5">
+        <v>19.2</v>
+      </c>
+      <c r="K56" s="5">
+        <v>19.5</v>
+      </c>
+      <c r="L56" s="5">
+        <v>19.8</v>
+      </c>
+      <c r="M56" s="5">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="N56" s="5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="O56" s="5">
+        <v>20.7</v>
+      </c>
+      <c r="P56" s="5">
+        <v>21</v>
+      </c>
+      <c r="Q56" s="5">
+        <v>21.3</v>
+      </c>
+      <c r="R56" s="5">
+        <v>21.6</v>
       </c>
     </row>
     <row r="57" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2684,38 +2684,38 @@
       <c r="G57" s="5">
         <v>18.5</v>
       </c>
-      <c r="H57" s="4">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="I57" s="4">
-        <v>20.7</v>
-      </c>
-      <c r="J57" s="4">
-        <v>21</v>
-      </c>
-      <c r="K57" s="4">
-        <v>21.3</v>
-      </c>
-      <c r="L57" s="4">
-        <v>21.6</v>
-      </c>
-      <c r="M57" s="4">
-        <v>21.9</v>
-      </c>
-      <c r="N57" s="4">
-        <v>22.1</v>
-      </c>
-      <c r="O57" s="4">
-        <v>22.3</v>
-      </c>
-      <c r="P57" s="4">
-        <v>22.5</v>
-      </c>
-      <c r="Q57" s="4">
-        <v>22.7</v>
-      </c>
-      <c r="R57" s="4">
-        <v>22.9</v>
+      <c r="H57" s="5">
+        <v>18.8</v>
+      </c>
+      <c r="I57" s="5">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="J57" s="5">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="K57" s="5">
+        <v>19.7</v>
+      </c>
+      <c r="L57" s="5">
+        <v>20</v>
+      </c>
+      <c r="M57" s="5">
+        <v>20.3</v>
+      </c>
+      <c r="N57" s="5">
+        <v>20.6</v>
+      </c>
+      <c r="O57" s="5">
+        <v>20.9</v>
+      </c>
+      <c r="P57" s="5">
+        <v>21.2</v>
+      </c>
+      <c r="Q57" s="5">
+        <v>21.5</v>
+      </c>
+      <c r="R57" s="5">
+        <v>21.8</v>
       </c>
     </row>
     <row r="58" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2737,38 +2737,38 @@
       <c r="G58" s="5">
         <v>18.7</v>
       </c>
-      <c r="H58" s="4">
+      <c r="H58" s="5">
+        <v>19</v>
+      </c>
+      <c r="I58" s="5">
+        <v>19.3</v>
+      </c>
+      <c r="J58" s="5">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K58" s="5">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="L58" s="5">
+        <v>20.2</v>
+      </c>
+      <c r="M58" s="5">
         <v>20.5</v>
       </c>
-      <c r="I58" s="4">
+      <c r="N58" s="5">
         <v>20.8</v>
       </c>
-      <c r="J58" s="4">
+      <c r="O58" s="5">
         <v>21.1</v>
       </c>
-      <c r="K58" s="4">
+      <c r="P58" s="5">
         <v>21.4</v>
       </c>
-      <c r="L58" s="4">
+      <c r="Q58" s="5">
         <v>21.7</v>
       </c>
-      <c r="M58" s="4">
+      <c r="R58" s="5">
         <v>22</v>
-      </c>
-      <c r="N58" s="4">
-        <v>22.2</v>
-      </c>
-      <c r="O58" s="4">
-        <v>22.4</v>
-      </c>
-      <c r="P58" s="4">
-        <v>22.6</v>
-      </c>
-      <c r="Q58" s="4">
-        <v>22.8</v>
-      </c>
-      <c r="R58" s="4">
-        <v>23</v>
       </c>
     </row>
     <row r="59" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2790,38 +2790,38 @@
       <c r="G59" s="5">
         <v>18.899999999999999</v>
       </c>
-      <c r="H59" s="4">
-        <v>20.6</v>
-      </c>
-      <c r="I59" s="4">
-        <v>20.9</v>
-      </c>
-      <c r="J59" s="4">
-        <v>21.2</v>
-      </c>
-      <c r="K59" s="4">
-        <v>21.5</v>
-      </c>
-      <c r="L59" s="4">
-        <v>21.8</v>
-      </c>
-      <c r="M59" s="4">
-        <v>22.1</v>
-      </c>
-      <c r="N59" s="4">
-        <v>22.3</v>
-      </c>
-      <c r="O59" s="4">
-        <v>22.5</v>
-      </c>
-      <c r="P59" s="4">
-        <v>22.7</v>
-      </c>
-      <c r="Q59" s="4">
-        <v>22.9</v>
-      </c>
-      <c r="R59" s="4">
-        <v>23.1</v>
+      <c r="H59" s="5">
+        <v>19.2</v>
+      </c>
+      <c r="I59" s="5">
+        <v>19.5</v>
+      </c>
+      <c r="J59" s="5">
+        <v>19.8</v>
+      </c>
+      <c r="K59" s="5">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L59" s="5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="M59" s="5">
+        <v>20.7</v>
+      </c>
+      <c r="N59" s="5">
+        <v>21</v>
+      </c>
+      <c r="O59" s="5">
+        <v>21.3</v>
+      </c>
+      <c r="P59" s="5">
+        <v>21.6</v>
+      </c>
+      <c r="Q59" s="5">
+        <v>21.9</v>
+      </c>
+      <c r="R59" s="5">
+        <v>22.2</v>
       </c>
     </row>
     <row r="60" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2843,38 +2843,38 @@
       <c r="G60" s="5">
         <v>19.100000000000001</v>
       </c>
-      <c r="H60" s="4">
-        <v>20.7</v>
-      </c>
-      <c r="I60" s="4">
-        <v>21</v>
-      </c>
-      <c r="J60" s="4">
-        <v>21.3</v>
-      </c>
-      <c r="K60" s="4">
-        <v>21.6</v>
-      </c>
-      <c r="L60" s="4">
-        <v>21.9</v>
-      </c>
-      <c r="M60" s="4">
-        <v>22.2</v>
-      </c>
-      <c r="N60" s="4">
+      <c r="H60" s="5">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="I60" s="5">
+        <v>19.7</v>
+      </c>
+      <c r="J60" s="5">
+        <v>20</v>
+      </c>
+      <c r="K60" s="5">
+        <v>20.3</v>
+      </c>
+      <c r="L60" s="5">
+        <v>20.6</v>
+      </c>
+      <c r="M60" s="5">
+        <v>20.9</v>
+      </c>
+      <c r="N60" s="5">
+        <v>21.2</v>
+      </c>
+      <c r="O60" s="5">
+        <v>21.5</v>
+      </c>
+      <c r="P60" s="5">
+        <v>21.8</v>
+      </c>
+      <c r="Q60" s="5">
+        <v>22.1</v>
+      </c>
+      <c r="R60" s="5">
         <v>22.4</v>
-      </c>
-      <c r="O60" s="4">
-        <v>22.6</v>
-      </c>
-      <c r="P60" s="4">
-        <v>22.8</v>
-      </c>
-      <c r="Q60" s="4">
-        <v>23</v>
-      </c>
-      <c r="R60" s="4">
-        <v>23.2</v>
       </c>
     </row>
     <row r="61" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2896,38 +2896,38 @@
       <c r="G61" s="5">
         <v>19.3</v>
       </c>
-      <c r="H61" s="4">
+      <c r="H61" s="5">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="I61" s="5">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="J61" s="5">
+        <v>20.2</v>
+      </c>
+      <c r="K61" s="5">
+        <v>20.5</v>
+      </c>
+      <c r="L61" s="5">
         <v>20.8</v>
       </c>
-      <c r="I61" s="4">
+      <c r="M61" s="5">
         <v>21.1</v>
       </c>
-      <c r="J61" s="4">
+      <c r="N61" s="5">
         <v>21.4</v>
       </c>
-      <c r="K61" s="4">
+      <c r="O61" s="5">
         <v>21.7</v>
       </c>
-      <c r="L61" s="4">
+      <c r="P61" s="5">
         <v>22</v>
       </c>
-      <c r="M61" s="4">
+      <c r="Q61" s="5">
         <v>22.3</v>
       </c>
-      <c r="N61" s="4">
-        <v>22.5</v>
-      </c>
-      <c r="O61" s="4">
-        <v>22.7</v>
-      </c>
-      <c r="P61" s="4">
-        <v>22.9</v>
-      </c>
-      <c r="Q61" s="4">
-        <v>23.1</v>
-      </c>
-      <c r="R61" s="4">
-        <v>23.3</v>
+      <c r="R61" s="5">
+        <v>22.6</v>
       </c>
     </row>
     <row r="62" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2949,38 +2949,38 @@
       <c r="G62" s="5">
         <v>19.5</v>
       </c>
-      <c r="H62" s="4">
-        <v>20.9</v>
-      </c>
-      <c r="I62" s="4">
-        <v>21.2</v>
-      </c>
-      <c r="J62" s="4">
-        <v>21.5</v>
-      </c>
-      <c r="K62" s="4">
-        <v>21.8</v>
-      </c>
-      <c r="L62" s="4">
-        <v>22.1</v>
-      </c>
-      <c r="M62" s="4">
-        <v>22.4</v>
-      </c>
-      <c r="N62" s="4">
-        <v>22.6</v>
-      </c>
-      <c r="O62" s="4">
+      <c r="H62" s="5">
+        <v>19.8</v>
+      </c>
+      <c r="I62" s="5">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J62" s="5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K62" s="5">
+        <v>20.7</v>
+      </c>
+      <c r="L62" s="5">
+        <v>21</v>
+      </c>
+      <c r="M62" s="5">
+        <v>21.3</v>
+      </c>
+      <c r="N62" s="5">
+        <v>21.6</v>
+      </c>
+      <c r="O62" s="5">
+        <v>21.9</v>
+      </c>
+      <c r="P62" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="Q62" s="5">
+        <v>22.5</v>
+      </c>
+      <c r="R62" s="5">
         <v>22.8</v>
-      </c>
-      <c r="P62" s="4">
-        <v>23</v>
-      </c>
-      <c r="Q62" s="4">
-        <v>23.2</v>
-      </c>
-      <c r="R62" s="4">
-        <v>23.4</v>
       </c>
     </row>
     <row r="63" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3002,38 +3002,38 @@
       <c r="G63" s="5">
         <v>19.7</v>
       </c>
-      <c r="H63" s="4">
-        <v>21</v>
-      </c>
-      <c r="I63" s="4">
-        <v>21.3</v>
-      </c>
-      <c r="J63" s="4">
-        <v>21.6</v>
-      </c>
-      <c r="K63" s="4">
-        <v>21.9</v>
-      </c>
-      <c r="L63" s="4">
-        <v>22.2</v>
-      </c>
-      <c r="M63" s="4">
-        <v>22.5</v>
-      </c>
-      <c r="N63" s="4">
+      <c r="H63" s="5">
+        <v>20</v>
+      </c>
+      <c r="I63" s="5">
+        <v>20.3</v>
+      </c>
+      <c r="J63" s="5">
+        <v>20.6</v>
+      </c>
+      <c r="K63" s="5">
+        <v>20.9</v>
+      </c>
+      <c r="L63" s="5">
+        <v>21.2</v>
+      </c>
+      <c r="M63" s="5">
+        <v>21.5</v>
+      </c>
+      <c r="N63" s="5">
+        <v>21.8</v>
+      </c>
+      <c r="O63" s="5">
+        <v>22.1</v>
+      </c>
+      <c r="P63" s="5">
+        <v>22.4</v>
+      </c>
+      <c r="Q63" s="5">
         <v>22.7</v>
       </c>
-      <c r="O63" s="4">
-        <v>22.9</v>
-      </c>
-      <c r="P63" s="4">
-        <v>23.1</v>
-      </c>
-      <c r="Q63" s="4">
-        <v>23.3</v>
-      </c>
-      <c r="R63" s="4">
-        <v>23.5</v>
+      <c r="R63" s="5">
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3055,38 +3055,38 @@
       <c r="G64" s="5">
         <v>19.899999999999999</v>
       </c>
-      <c r="H64" s="4">
+      <c r="H64" s="5">
+        <v>20.2</v>
+      </c>
+      <c r="I64" s="5">
+        <v>20.5</v>
+      </c>
+      <c r="J64" s="5">
+        <v>20.8</v>
+      </c>
+      <c r="K64" s="5">
         <v>21.1</v>
       </c>
-      <c r="I64" s="4">
+      <c r="L64" s="5">
         <v>21.4</v>
       </c>
-      <c r="J64" s="4">
+      <c r="M64" s="5">
         <v>21.7</v>
       </c>
-      <c r="K64" s="4">
+      <c r="N64" s="5">
         <v>22</v>
       </c>
-      <c r="L64" s="4">
+      <c r="O64" s="5">
         <v>22.3</v>
       </c>
-      <c r="M64" s="4">
+      <c r="P64" s="5">
         <v>22.6</v>
       </c>
-      <c r="N64" s="4">
-        <v>22.8</v>
-      </c>
-      <c r="O64" s="4">
-        <v>23</v>
-      </c>
-      <c r="P64" s="4">
+      <c r="Q64" s="5">
+        <v>22.9</v>
+      </c>
+      <c r="R64" s="5">
         <v>23.2</v>
-      </c>
-      <c r="Q64" s="4">
-        <v>23.4</v>
-      </c>
-      <c r="R64" s="4">
-        <v>23.6</v>
       </c>
     </row>
     <row r="65" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3108,38 +3108,38 @@
       <c r="G65" s="5">
         <v>20.100000000000001</v>
       </c>
-      <c r="H65" s="4">
-        <v>21.2</v>
-      </c>
-      <c r="I65" s="4">
-        <v>21.5</v>
-      </c>
-      <c r="J65" s="4">
-        <v>21.8</v>
-      </c>
-      <c r="K65" s="4">
-        <v>22.1</v>
-      </c>
-      <c r="L65" s="4">
-        <v>22.4</v>
-      </c>
-      <c r="M65" s="4">
-        <v>22.7</v>
-      </c>
-      <c r="N65" s="4">
-        <v>22.9</v>
-      </c>
-      <c r="O65" s="4">
+      <c r="H65" s="5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="I65" s="5">
+        <v>20.7</v>
+      </c>
+      <c r="J65" s="5">
+        <v>21</v>
+      </c>
+      <c r="K65" s="5">
+        <v>21.3</v>
+      </c>
+      <c r="L65" s="5">
+        <v>21.6</v>
+      </c>
+      <c r="M65" s="5">
+        <v>21.9</v>
+      </c>
+      <c r="N65" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="O65" s="5">
+        <v>22.5</v>
+      </c>
+      <c r="P65" s="5">
+        <v>22.8</v>
+      </c>
+      <c r="Q65" s="5">
         <v>23.1</v>
       </c>
-      <c r="P65" s="4">
-        <v>23.3</v>
-      </c>
-      <c r="Q65" s="4">
-        <v>23.5</v>
-      </c>
-      <c r="R65" s="4">
-        <v>23.7</v>
+      <c r="R65" s="5">
+        <v>23.4</v>
       </c>
     </row>
     <row r="66" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3161,38 +3161,38 @@
       <c r="G66" s="5">
         <v>20.3</v>
       </c>
-      <c r="H66" s="4">
-        <v>21.3</v>
-      </c>
-      <c r="I66" s="4">
-        <v>21.6</v>
-      </c>
-      <c r="J66" s="4">
-        <v>21.9</v>
-      </c>
-      <c r="K66" s="4">
-        <v>22.2</v>
-      </c>
-      <c r="L66" s="4">
-        <v>22.5</v>
-      </c>
-      <c r="M66" s="4">
-        <v>22.8</v>
-      </c>
-      <c r="N66" s="4">
+      <c r="H66" s="5">
+        <v>20.6</v>
+      </c>
+      <c r="I66" s="5">
+        <v>20.9</v>
+      </c>
+      <c r="J66" s="5">
+        <v>21.2</v>
+      </c>
+      <c r="K66" s="5">
+        <v>21.5</v>
+      </c>
+      <c r="L66" s="5">
+        <v>21.8</v>
+      </c>
+      <c r="M66" s="5">
+        <v>22.1</v>
+      </c>
+      <c r="N66" s="5">
+        <v>22.4</v>
+      </c>
+      <c r="O66" s="5">
+        <v>22.7</v>
+      </c>
+      <c r="P66" s="5">
         <v>23</v>
       </c>
-      <c r="O66" s="4">
-        <v>23.2</v>
-      </c>
-      <c r="P66" s="4">
-        <v>23.4</v>
-      </c>
-      <c r="Q66" s="4">
+      <c r="Q66" s="5">
+        <v>23.3</v>
+      </c>
+      <c r="R66" s="5">
         <v>23.6</v>
-      </c>
-      <c r="R66" s="4">
-        <v>23.8</v>
       </c>
     </row>
     <row r="67" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3214,38 +3214,38 @@
       <c r="G67" s="5">
         <v>20.5</v>
       </c>
-      <c r="H67" s="4">
+      <c r="H67" s="5">
+        <v>20.8</v>
+      </c>
+      <c r="I67" s="5">
+        <v>21.1</v>
+      </c>
+      <c r="J67" s="5">
         <v>21.4</v>
       </c>
-      <c r="I67" s="4">
+      <c r="K67" s="5">
         <v>21.7</v>
       </c>
-      <c r="J67" s="4">
+      <c r="L67" s="5">
         <v>22</v>
       </c>
-      <c r="K67" s="4">
+      <c r="M67" s="5">
         <v>22.3</v>
       </c>
-      <c r="L67" s="4">
+      <c r="N67" s="5">
         <v>22.6</v>
       </c>
-      <c r="M67" s="4">
+      <c r="O67" s="5">
         <v>22.9</v>
       </c>
-      <c r="N67" s="4">
-        <v>23.1</v>
-      </c>
-      <c r="O67" s="4">
-        <v>23.3</v>
-      </c>
-      <c r="P67" s="4">
+      <c r="P67" s="5">
+        <v>23.2</v>
+      </c>
+      <c r="Q67" s="5">
         <v>23.5</v>
       </c>
-      <c r="Q67" s="4">
-        <v>23.7</v>
-      </c>
-      <c r="R67" s="4">
-        <v>23.9</v>
+      <c r="R67" s="5">
+        <v>23.8</v>
       </c>
     </row>
     <row r="68" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3267,37 +3267,37 @@
       <c r="G68" s="5">
         <v>20.7</v>
       </c>
-      <c r="H68" s="4">
-        <v>21.5</v>
-      </c>
-      <c r="I68" s="4">
-        <v>21.8</v>
-      </c>
-      <c r="J68" s="4">
-        <v>22.1</v>
-      </c>
-      <c r="K68" s="4">
-        <v>22.4</v>
-      </c>
-      <c r="L68" s="4">
-        <v>22.7</v>
-      </c>
-      <c r="M68" s="4">
-        <v>23</v>
-      </c>
-      <c r="N68" s="4">
-        <v>23.2</v>
-      </c>
-      <c r="O68" s="4">
+      <c r="H68" s="5">
+        <v>21</v>
+      </c>
+      <c r="I68" s="5">
+        <v>21.3</v>
+      </c>
+      <c r="J68" s="5">
+        <v>21.6</v>
+      </c>
+      <c r="K68" s="5">
+        <v>21.9</v>
+      </c>
+      <c r="L68" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="M68" s="5">
+        <v>22.5</v>
+      </c>
+      <c r="N68" s="5">
+        <v>22.8</v>
+      </c>
+      <c r="O68" s="5">
+        <v>23.1</v>
+      </c>
+      <c r="P68" s="5">
         <v>23.4</v>
       </c>
-      <c r="P68" s="4">
-        <v>23.6</v>
-      </c>
-      <c r="Q68" s="4">
-        <v>23.8</v>
-      </c>
-      <c r="R68" s="4">
+      <c r="Q68" s="5">
+        <v>23.7</v>
+      </c>
+      <c r="R68" s="5">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Laxman : Milk rate chart paste button made work
</commit_message>
<xml_diff>
--- a/Milk_Rate_Chart_Template.xlsx
+++ b/Milk_Rate_Chart_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Products\LPMilkDairyFirm\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA27714A-9C9F-420E-8817-43E09E139E3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -308,14 +309,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B3:R69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43:R68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1942,38 +1943,38 @@
       <c r="G43" s="5">
         <v>14.2</v>
       </c>
-      <c r="H43" s="5">
-        <v>14.5</v>
-      </c>
-      <c r="I43" s="5">
-        <v>14.8</v>
-      </c>
-      <c r="J43" s="5">
-        <v>15.1</v>
-      </c>
-      <c r="K43" s="5">
-        <v>15.4</v>
-      </c>
-      <c r="L43" s="5">
-        <v>15.7</v>
-      </c>
-      <c r="M43" s="5">
-        <v>16</v>
-      </c>
-      <c r="N43" s="5">
-        <v>16.3</v>
-      </c>
-      <c r="O43" s="5">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="P43" s="5">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="Q43" s="5">
-        <v>17.2</v>
-      </c>
-      <c r="R43" s="5">
-        <v>17.5</v>
+      <c r="H43" s="4">
+        <v>18</v>
+      </c>
+      <c r="I43" s="4">
+        <v>18.3</v>
+      </c>
+      <c r="J43" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="K43" s="4">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="L43" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="M43" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="N43" s="4">
+        <v>19.7</v>
+      </c>
+      <c r="O43" s="4">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="P43" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="Q43" s="4">
+        <v>20.3</v>
+      </c>
+      <c r="R43" s="4">
+        <v>20.5</v>
       </c>
     </row>
     <row r="44" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1995,38 +1996,38 @@
       <c r="G44" s="5">
         <v>14.7</v>
       </c>
-      <c r="H44" s="5">
-        <v>15</v>
-      </c>
-      <c r="I44" s="5">
-        <v>15.3</v>
-      </c>
-      <c r="J44" s="5">
-        <v>15.6</v>
-      </c>
-      <c r="K44" s="5">
-        <v>15.9</v>
-      </c>
-      <c r="L44" s="5">
-        <v>16.2</v>
-      </c>
-      <c r="M44" s="5">
-        <v>16.5</v>
-      </c>
-      <c r="N44" s="5">
-        <v>16.8</v>
-      </c>
-      <c r="O44" s="5">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="P44" s="5">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="Q44" s="5">
-        <v>17.7</v>
-      </c>
-      <c r="R44" s="5">
-        <v>18</v>
+      <c r="H44" s="4">
+        <v>18.3</v>
+      </c>
+      <c r="I44" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="J44" s="4">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="K44" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="L44" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="M44" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="N44" s="4">
+        <v>20</v>
+      </c>
+      <c r="O44" s="4">
+        <v>20.2</v>
+      </c>
+      <c r="P44" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="R44" s="4">
+        <v>20.8</v>
       </c>
     </row>
     <row r="45" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2048,38 +2049,38 @@
       <c r="G45" s="5">
         <v>15.2</v>
       </c>
-      <c r="H45" s="5">
-        <v>15.5</v>
-      </c>
-      <c r="I45" s="5">
-        <v>15.8</v>
-      </c>
-      <c r="J45" s="5">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="K45" s="5">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="L45" s="5">
-        <v>16.7</v>
-      </c>
-      <c r="M45" s="5">
-        <v>17</v>
-      </c>
-      <c r="N45" s="5">
-        <v>17.3</v>
-      </c>
-      <c r="O45" s="5">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="P45" s="5">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="Q45" s="5">
-        <v>18.2</v>
-      </c>
-      <c r="R45" s="5">
-        <v>18.5</v>
+      <c r="H45" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="I45" s="4">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J45" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="K45" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="L45" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="M45" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="N45" s="4">
+        <v>20.3</v>
+      </c>
+      <c r="O45" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="P45" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="Q45" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="R45" s="4">
+        <v>21.1</v>
       </c>
     </row>
     <row r="46" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2101,38 +2102,38 @@
       <c r="G46" s="5">
         <v>15.7</v>
       </c>
-      <c r="H46" s="5">
-        <v>16</v>
-      </c>
-      <c r="I46" s="5">
-        <v>16.3</v>
-      </c>
-      <c r="J46" s="5">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="K46" s="5">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="L46" s="5">
-        <v>17.2</v>
-      </c>
-      <c r="M46" s="5">
-        <v>17.5</v>
-      </c>
-      <c r="N46" s="5">
-        <v>17.8</v>
-      </c>
-      <c r="O46" s="5">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="P46" s="5">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="Q46" s="5">
-        <v>18.7</v>
-      </c>
-      <c r="R46" s="5">
-        <v>19</v>
+      <c r="H46" s="4">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="I46" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="J46" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="K46" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="L46" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="M46" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="N46" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="O46" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="P46" s="4">
+        <v>21</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="R46" s="4">
+        <v>21.4</v>
       </c>
     </row>
     <row r="47" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2154,38 +2155,38 @@
       <c r="G47" s="5">
         <v>16.2</v>
       </c>
-      <c r="H47" s="5">
-        <v>16.5</v>
-      </c>
-      <c r="I47" s="5">
-        <v>16.8</v>
-      </c>
-      <c r="J47" s="5">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="K47" s="5">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="L47" s="5">
-        <v>17.7</v>
-      </c>
-      <c r="M47" s="5">
-        <v>18</v>
-      </c>
-      <c r="N47" s="5">
-        <v>18.3</v>
-      </c>
-      <c r="O47" s="5">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="P47" s="5">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="Q47" s="5">
+      <c r="H47" s="4">
         <v>19.2</v>
       </c>
-      <c r="R47" s="5">
+      <c r="I47" s="4">
         <v>19.5</v>
+      </c>
+      <c r="J47" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="K47" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L47" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="M47" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="N47" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="O47" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="P47" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="R47" s="4">
+        <v>21.7</v>
       </c>
     </row>
     <row r="48" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2207,38 +2208,38 @@
       <c r="G48" s="5">
         <v>16.7</v>
       </c>
-      <c r="H48" s="5">
-        <v>17</v>
-      </c>
-      <c r="I48" s="5">
-        <v>17.3</v>
-      </c>
-      <c r="J48" s="5">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="K48" s="5">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="L48" s="5">
-        <v>18.2</v>
-      </c>
-      <c r="M48" s="5">
-        <v>18.5</v>
-      </c>
-      <c r="N48" s="5">
-        <v>18.8</v>
-      </c>
-      <c r="O48" s="5">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="P48" s="5">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="Q48" s="5">
-        <v>19.7</v>
-      </c>
-      <c r="R48" s="5">
-        <v>20</v>
+      <c r="H48" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="I48" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="J48" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="K48" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="L48" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="M48" s="4">
+        <v>21</v>
+      </c>
+      <c r="N48" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="O48" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="P48" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="R48" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2260,38 +2261,38 @@
       <c r="G49" s="5">
         <v>16.899999999999999</v>
       </c>
-      <c r="H49" s="6">
-        <v>17.2</v>
-      </c>
-      <c r="I49" s="5">
-        <v>17.5</v>
-      </c>
-      <c r="J49" s="5">
-        <v>17.8</v>
-      </c>
-      <c r="K49" s="5">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="L49" s="5">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="M49" s="6">
-        <v>18.7</v>
-      </c>
-      <c r="N49" s="5">
-        <v>19</v>
-      </c>
-      <c r="O49" s="5">
-        <v>19.3</v>
-      </c>
-      <c r="P49" s="5">
+      <c r="H49" s="4">
         <v>19.600000000000001</v>
       </c>
-      <c r="Q49" s="5">
+      <c r="I49" s="4">
         <v>19.899999999999999</v>
       </c>
-      <c r="R49" s="6">
+      <c r="J49" s="4">
         <v>20.2</v>
+      </c>
+      <c r="K49" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="L49" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="M49" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="N49" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="O49" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="P49" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="R49" s="4">
+        <v>22.1</v>
       </c>
     </row>
     <row r="50" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2313,38 +2314,38 @@
       <c r="G50" s="5">
         <v>17.100000000000001</v>
       </c>
-      <c r="H50" s="5">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="I50" s="5">
-        <v>17.7</v>
-      </c>
-      <c r="J50" s="5">
-        <v>18</v>
-      </c>
-      <c r="K50" s="5">
-        <v>18.3</v>
-      </c>
-      <c r="L50" s="5">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="M50" s="5">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="N50" s="5">
-        <v>19.2</v>
-      </c>
-      <c r="O50" s="5">
-        <v>19.5</v>
-      </c>
-      <c r="P50" s="5">
-        <v>19.8</v>
-      </c>
-      <c r="Q50" s="5">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="R50" s="5">
-        <v>20.399999999999999</v>
+      <c r="H50" s="4">
+        <v>19.7</v>
+      </c>
+      <c r="I50" s="4">
+        <v>20</v>
+      </c>
+      <c r="J50" s="4">
+        <v>20.3</v>
+      </c>
+      <c r="K50" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="L50" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="M50" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="N50" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="O50" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="P50" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>22</v>
+      </c>
+      <c r="R50" s="4">
+        <v>22.2</v>
       </c>
     </row>
     <row r="51" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2366,38 +2367,38 @@
       <c r="G51" s="5">
         <v>17.3</v>
       </c>
-      <c r="H51" s="5">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="I51" s="5">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="J51" s="5">
-        <v>18.2</v>
-      </c>
-      <c r="K51" s="5">
-        <v>18.5</v>
-      </c>
-      <c r="L51" s="5">
-        <v>18.8</v>
-      </c>
-      <c r="M51" s="5">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="N51" s="5">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="O51" s="5">
-        <v>19.7</v>
-      </c>
-      <c r="P51" s="5">
-        <v>20</v>
-      </c>
-      <c r="Q51" s="5">
-        <v>20.3</v>
-      </c>
-      <c r="R51" s="5">
-        <v>20.6</v>
+      <c r="H51" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="I51" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J51" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K51" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="L51" s="4">
+        <v>21</v>
+      </c>
+      <c r="M51" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="N51" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="O51" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="P51" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="R51" s="4">
+        <v>22.3</v>
       </c>
     </row>
     <row r="52" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2419,38 +2420,38 @@
       <c r="G52" s="5">
         <v>17.5</v>
       </c>
-      <c r="H52" s="5">
-        <v>17.8</v>
-      </c>
-      <c r="I52" s="5">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="J52" s="5">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="K52" s="5">
-        <v>18.7</v>
-      </c>
-      <c r="L52" s="5">
-        <v>19</v>
-      </c>
-      <c r="M52" s="5">
-        <v>19.3</v>
-      </c>
-      <c r="N52" s="5">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="O52" s="5">
+      <c r="H52" s="4">
         <v>19.899999999999999</v>
       </c>
-      <c r="P52" s="5">
+      <c r="I52" s="4">
         <v>20.2</v>
       </c>
-      <c r="Q52" s="5">
+      <c r="J52" s="4">
         <v>20.5</v>
       </c>
-      <c r="R52" s="5">
+      <c r="K52" s="4">
         <v>20.8</v>
+      </c>
+      <c r="L52" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="M52" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="N52" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="O52" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="P52" s="4">
+        <v>22</v>
+      </c>
+      <c r="Q52" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="R52" s="4">
+        <v>22.4</v>
       </c>
     </row>
     <row r="53" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2472,38 +2473,38 @@
       <c r="G53" s="5">
         <v>17.7</v>
       </c>
-      <c r="H53" s="5">
-        <v>18</v>
-      </c>
-      <c r="I53" s="5">
-        <v>18.3</v>
-      </c>
-      <c r="J53" s="5">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="K53" s="5">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="L53" s="5">
-        <v>19.2</v>
-      </c>
-      <c r="M53" s="5">
-        <v>19.5</v>
-      </c>
-      <c r="N53" s="5">
-        <v>19.8</v>
-      </c>
-      <c r="O53" s="5">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="P53" s="5">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="Q53" s="5">
-        <v>20.7</v>
-      </c>
-      <c r="R53" s="5">
-        <v>21</v>
+      <c r="H53" s="4">
+        <v>20</v>
+      </c>
+      <c r="I53" s="4">
+        <v>20.3</v>
+      </c>
+      <c r="J53" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="K53" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="L53" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="M53" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="N53" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="O53" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="P53" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="R53" s="4">
+        <v>22.5</v>
       </c>
     </row>
     <row r="54" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2525,38 +2526,38 @@
       <c r="G54" s="5">
         <v>17.899999999999999</v>
       </c>
-      <c r="H54" s="5">
-        <v>18.2</v>
-      </c>
-      <c r="I54" s="5">
-        <v>18.5</v>
-      </c>
-      <c r="J54" s="5">
-        <v>18.8</v>
-      </c>
-      <c r="K54" s="5">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="L54" s="5">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="M54" s="5">
-        <v>19.7</v>
-      </c>
-      <c r="N54" s="5">
-        <v>20</v>
-      </c>
-      <c r="O54" s="5">
-        <v>20.3</v>
-      </c>
-      <c r="P54" s="5">
-        <v>20.6</v>
-      </c>
-      <c r="Q54" s="5">
-        <v>20.9</v>
-      </c>
-      <c r="R54" s="5">
-        <v>21.2</v>
+      <c r="H54" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I54" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J54" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="K54" s="4">
+        <v>21</v>
+      </c>
+      <c r="L54" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="M54" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="N54" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="O54" s="4">
+        <v>22</v>
+      </c>
+      <c r="P54" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="R54" s="4">
+        <v>22.6</v>
       </c>
     </row>
     <row r="55" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2578,38 +2579,38 @@
       <c r="G55" s="5">
         <v>18.100000000000001</v>
       </c>
-      <c r="H55" s="5">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="I55" s="5">
-        <v>18.7</v>
-      </c>
-      <c r="J55" s="5">
-        <v>19</v>
-      </c>
-      <c r="K55" s="5">
-        <v>19.3</v>
-      </c>
-      <c r="L55" s="5">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="M55" s="5">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="N55" s="5">
+      <c r="H55" s="4">
         <v>20.2</v>
       </c>
-      <c r="O55" s="5">
+      <c r="I55" s="4">
         <v>20.5</v>
       </c>
-      <c r="P55" s="5">
+      <c r="J55" s="4">
         <v>20.8</v>
       </c>
-      <c r="Q55" s="5">
+      <c r="K55" s="4">
         <v>21.1</v>
       </c>
-      <c r="R55" s="5">
+      <c r="L55" s="4">
         <v>21.4</v>
+      </c>
+      <c r="M55" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="N55" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="O55" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="P55" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="R55" s="4">
+        <v>22.7</v>
       </c>
     </row>
     <row r="56" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2631,38 +2632,38 @@
       <c r="G56" s="5">
         <v>18.3</v>
       </c>
-      <c r="H56" s="5">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="I56" s="5">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="J56" s="5">
-        <v>19.2</v>
-      </c>
-      <c r="K56" s="5">
-        <v>19.5</v>
-      </c>
-      <c r="L56" s="5">
-        <v>19.8</v>
-      </c>
-      <c r="M56" s="5">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="N56" s="5">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="O56" s="5">
-        <v>20.7</v>
-      </c>
-      <c r="P56" s="5">
-        <v>21</v>
-      </c>
-      <c r="Q56" s="5">
-        <v>21.3</v>
-      </c>
-      <c r="R56" s="5">
-        <v>21.6</v>
+      <c r="H56" s="4">
+        <v>20.3</v>
+      </c>
+      <c r="I56" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="J56" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="K56" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="L56" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="M56" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="N56" s="4">
+        <v>22</v>
+      </c>
+      <c r="O56" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="P56" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="Q56" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="R56" s="4">
+        <v>22.8</v>
       </c>
     </row>
     <row r="57" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2684,38 +2685,38 @@
       <c r="G57" s="5">
         <v>18.5</v>
       </c>
-      <c r="H57" s="5">
-        <v>18.8</v>
-      </c>
-      <c r="I57" s="5">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="J57" s="5">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="K57" s="5">
-        <v>19.7</v>
-      </c>
-      <c r="L57" s="5">
-        <v>20</v>
-      </c>
-      <c r="M57" s="5">
-        <v>20.3</v>
-      </c>
-      <c r="N57" s="5">
-        <v>20.6</v>
-      </c>
-      <c r="O57" s="5">
-        <v>20.9</v>
-      </c>
-      <c r="P57" s="5">
-        <v>21.2</v>
-      </c>
-      <c r="Q57" s="5">
-        <v>21.5</v>
-      </c>
-      <c r="R57" s="5">
-        <v>21.8</v>
+      <c r="H57" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="I57" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="J57" s="4">
+        <v>21</v>
+      </c>
+      <c r="K57" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="L57" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="M57" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="N57" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="O57" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="P57" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="Q57" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="R57" s="4">
+        <v>22.9</v>
       </c>
     </row>
     <row r="58" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2737,38 +2738,38 @@
       <c r="G58" s="5">
         <v>18.7</v>
       </c>
-      <c r="H58" s="5">
-        <v>19</v>
-      </c>
-      <c r="I58" s="5">
-        <v>19.3</v>
-      </c>
-      <c r="J58" s="5">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="K58" s="5">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="L58" s="5">
-        <v>20.2</v>
-      </c>
-      <c r="M58" s="5">
+      <c r="H58" s="4">
         <v>20.5</v>
       </c>
-      <c r="N58" s="5">
+      <c r="I58" s="4">
         <v>20.8</v>
       </c>
-      <c r="O58" s="5">
+      <c r="J58" s="4">
         <v>21.1</v>
       </c>
-      <c r="P58" s="5">
+      <c r="K58" s="4">
         <v>21.4</v>
       </c>
-      <c r="Q58" s="5">
+      <c r="L58" s="4">
         <v>21.7</v>
       </c>
-      <c r="R58" s="5">
+      <c r="M58" s="4">
         <v>22</v>
+      </c>
+      <c r="N58" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="O58" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="P58" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="Q58" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="R58" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2790,38 +2791,38 @@
       <c r="G59" s="5">
         <v>18.899999999999999</v>
       </c>
-      <c r="H59" s="5">
-        <v>19.2</v>
-      </c>
-      <c r="I59" s="5">
-        <v>19.5</v>
-      </c>
-      <c r="J59" s="5">
-        <v>19.8</v>
-      </c>
-      <c r="K59" s="5">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L59" s="5">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="M59" s="5">
-        <v>20.7</v>
-      </c>
-      <c r="N59" s="5">
-        <v>21</v>
-      </c>
-      <c r="O59" s="5">
-        <v>21.3</v>
-      </c>
-      <c r="P59" s="5">
-        <v>21.6</v>
-      </c>
-      <c r="Q59" s="5">
-        <v>21.9</v>
-      </c>
-      <c r="R59" s="5">
-        <v>22.2</v>
+      <c r="H59" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="I59" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="J59" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="K59" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="L59" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="M59" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="N59" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="O59" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="P59" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="Q59" s="4">
+        <v>22.9</v>
+      </c>
+      <c r="R59" s="4">
+        <v>23.1</v>
       </c>
     </row>
     <row r="60" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2843,38 +2844,38 @@
       <c r="G60" s="5">
         <v>19.100000000000001</v>
       </c>
-      <c r="H60" s="5">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="I60" s="5">
-        <v>19.7</v>
-      </c>
-      <c r="J60" s="5">
-        <v>20</v>
-      </c>
-      <c r="K60" s="5">
-        <v>20.3</v>
-      </c>
-      <c r="L60" s="5">
-        <v>20.6</v>
-      </c>
-      <c r="M60" s="5">
-        <v>20.9</v>
-      </c>
-      <c r="N60" s="5">
-        <v>21.2</v>
-      </c>
-      <c r="O60" s="5">
-        <v>21.5</v>
-      </c>
-      <c r="P60" s="5">
-        <v>21.8</v>
-      </c>
-      <c r="Q60" s="5">
-        <v>22.1</v>
-      </c>
-      <c r="R60" s="5">
+      <c r="H60" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="I60" s="4">
+        <v>21</v>
+      </c>
+      <c r="J60" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="K60" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="L60" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="M60" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="N60" s="4">
         <v>22.4</v>
+      </c>
+      <c r="O60" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="P60" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="Q60" s="4">
+        <v>23</v>
+      </c>
+      <c r="R60" s="4">
+        <v>23.2</v>
       </c>
     </row>
     <row r="61" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2896,38 +2897,38 @@
       <c r="G61" s="5">
         <v>19.3</v>
       </c>
-      <c r="H61" s="5">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I61" s="5">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="J61" s="5">
-        <v>20.2</v>
-      </c>
-      <c r="K61" s="5">
-        <v>20.5</v>
-      </c>
-      <c r="L61" s="5">
+      <c r="H61" s="4">
         <v>20.8</v>
       </c>
-      <c r="M61" s="5">
+      <c r="I61" s="4">
         <v>21.1</v>
       </c>
-      <c r="N61" s="5">
+      <c r="J61" s="4">
         <v>21.4</v>
       </c>
-      <c r="O61" s="5">
+      <c r="K61" s="4">
         <v>21.7</v>
       </c>
-      <c r="P61" s="5">
+      <c r="L61" s="4">
         <v>22</v>
       </c>
-      <c r="Q61" s="5">
+      <c r="M61" s="4">
         <v>22.3</v>
       </c>
-      <c r="R61" s="5">
-        <v>22.6</v>
+      <c r="N61" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="O61" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="P61" s="4">
+        <v>22.9</v>
+      </c>
+      <c r="Q61" s="4">
+        <v>23.1</v>
+      </c>
+      <c r="R61" s="4">
+        <v>23.3</v>
       </c>
     </row>
     <row r="62" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2949,38 +2950,38 @@
       <c r="G62" s="5">
         <v>19.5</v>
       </c>
-      <c r="H62" s="5">
-        <v>19.8</v>
-      </c>
-      <c r="I62" s="5">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="J62" s="5">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="K62" s="5">
-        <v>20.7</v>
-      </c>
-      <c r="L62" s="5">
-        <v>21</v>
-      </c>
-      <c r="M62" s="5">
-        <v>21.3</v>
-      </c>
-      <c r="N62" s="5">
-        <v>21.6</v>
-      </c>
-      <c r="O62" s="5">
-        <v>21.9</v>
-      </c>
-      <c r="P62" s="5">
-        <v>22.2</v>
-      </c>
-      <c r="Q62" s="5">
-        <v>22.5</v>
-      </c>
-      <c r="R62" s="5">
+      <c r="H62" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="I62" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="J62" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="K62" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="L62" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="M62" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="N62" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="O62" s="4">
         <v>22.8</v>
+      </c>
+      <c r="P62" s="4">
+        <v>23</v>
+      </c>
+      <c r="Q62" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="R62" s="4">
+        <v>23.4</v>
       </c>
     </row>
     <row r="63" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3002,38 +3003,38 @@
       <c r="G63" s="5">
         <v>19.7</v>
       </c>
-      <c r="H63" s="5">
-        <v>20</v>
-      </c>
-      <c r="I63" s="5">
-        <v>20.3</v>
-      </c>
-      <c r="J63" s="5">
-        <v>20.6</v>
-      </c>
-      <c r="K63" s="5">
-        <v>20.9</v>
-      </c>
-      <c r="L63" s="5">
-        <v>21.2</v>
-      </c>
-      <c r="M63" s="5">
-        <v>21.5</v>
-      </c>
-      <c r="N63" s="5">
-        <v>21.8</v>
-      </c>
-      <c r="O63" s="5">
-        <v>22.1</v>
-      </c>
-      <c r="P63" s="5">
-        <v>22.4</v>
-      </c>
-      <c r="Q63" s="5">
+      <c r="H63" s="4">
+        <v>21</v>
+      </c>
+      <c r="I63" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="J63" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="K63" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="L63" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="M63" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="N63" s="4">
         <v>22.7</v>
       </c>
-      <c r="R63" s="5">
-        <v>23</v>
+      <c r="O63" s="4">
+        <v>22.9</v>
+      </c>
+      <c r="P63" s="4">
+        <v>23.1</v>
+      </c>
+      <c r="Q63" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="R63" s="4">
+        <v>23.5</v>
       </c>
     </row>
     <row r="64" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3055,38 +3056,38 @@
       <c r="G64" s="5">
         <v>19.899999999999999</v>
       </c>
-      <c r="H64" s="5">
-        <v>20.2</v>
-      </c>
-      <c r="I64" s="5">
-        <v>20.5</v>
-      </c>
-      <c r="J64" s="5">
-        <v>20.8</v>
-      </c>
-      <c r="K64" s="5">
+      <c r="H64" s="4">
         <v>21.1</v>
       </c>
-      <c r="L64" s="5">
+      <c r="I64" s="4">
         <v>21.4</v>
       </c>
-      <c r="M64" s="5">
+      <c r="J64" s="4">
         <v>21.7</v>
       </c>
-      <c r="N64" s="5">
+      <c r="K64" s="4">
         <v>22</v>
       </c>
-      <c r="O64" s="5">
+      <c r="L64" s="4">
         <v>22.3</v>
       </c>
-      <c r="P64" s="5">
+      <c r="M64" s="4">
         <v>22.6</v>
       </c>
-      <c r="Q64" s="5">
-        <v>22.9</v>
-      </c>
-      <c r="R64" s="5">
+      <c r="N64" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="O64" s="4">
+        <v>23</v>
+      </c>
+      <c r="P64" s="4">
         <v>23.2</v>
+      </c>
+      <c r="Q64" s="4">
+        <v>23.4</v>
+      </c>
+      <c r="R64" s="4">
+        <v>23.6</v>
       </c>
     </row>
     <row r="65" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3108,38 +3109,38 @@
       <c r="G65" s="5">
         <v>20.100000000000001</v>
       </c>
-      <c r="H65" s="5">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="I65" s="5">
-        <v>20.7</v>
-      </c>
-      <c r="J65" s="5">
-        <v>21</v>
-      </c>
-      <c r="K65" s="5">
-        <v>21.3</v>
-      </c>
-      <c r="L65" s="5">
-        <v>21.6</v>
-      </c>
-      <c r="M65" s="5">
-        <v>21.9</v>
-      </c>
-      <c r="N65" s="5">
-        <v>22.2</v>
-      </c>
-      <c r="O65" s="5">
-        <v>22.5</v>
-      </c>
-      <c r="P65" s="5">
-        <v>22.8</v>
-      </c>
-      <c r="Q65" s="5">
+      <c r="H65" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="I65" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="J65" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="K65" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="L65" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="M65" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="N65" s="4">
+        <v>22.9</v>
+      </c>
+      <c r="O65" s="4">
         <v>23.1</v>
       </c>
-      <c r="R65" s="5">
-        <v>23.4</v>
+      <c r="P65" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="Q65" s="4">
+        <v>23.5</v>
+      </c>
+      <c r="R65" s="4">
+        <v>23.7</v>
       </c>
     </row>
     <row r="66" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3161,38 +3162,38 @@
       <c r="G66" s="5">
         <v>20.3</v>
       </c>
-      <c r="H66" s="5">
-        <v>20.6</v>
-      </c>
-      <c r="I66" s="5">
-        <v>20.9</v>
-      </c>
-      <c r="J66" s="5">
-        <v>21.2</v>
-      </c>
-      <c r="K66" s="5">
-        <v>21.5</v>
-      </c>
-      <c r="L66" s="5">
-        <v>21.8</v>
-      </c>
-      <c r="M66" s="5">
-        <v>22.1</v>
-      </c>
-      <c r="N66" s="5">
-        <v>22.4</v>
-      </c>
-      <c r="O66" s="5">
-        <v>22.7</v>
-      </c>
-      <c r="P66" s="5">
+      <c r="H66" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="I66" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="J66" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="K66" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="L66" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="M66" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="N66" s="4">
         <v>23</v>
       </c>
-      <c r="Q66" s="5">
-        <v>23.3</v>
-      </c>
-      <c r="R66" s="5">
+      <c r="O66" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="P66" s="4">
+        <v>23.4</v>
+      </c>
+      <c r="Q66" s="4">
         <v>23.6</v>
+      </c>
+      <c r="R66" s="4">
+        <v>23.8</v>
       </c>
     </row>
     <row r="67" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3214,38 +3215,38 @@
       <c r="G67" s="5">
         <v>20.5</v>
       </c>
-      <c r="H67" s="5">
-        <v>20.8</v>
-      </c>
-      <c r="I67" s="5">
-        <v>21.1</v>
-      </c>
-      <c r="J67" s="5">
+      <c r="H67" s="4">
         <v>21.4</v>
       </c>
-      <c r="K67" s="5">
+      <c r="I67" s="4">
         <v>21.7</v>
       </c>
-      <c r="L67" s="5">
+      <c r="J67" s="4">
         <v>22</v>
       </c>
-      <c r="M67" s="5">
+      <c r="K67" s="4">
         <v>22.3</v>
       </c>
-      <c r="N67" s="5">
+      <c r="L67" s="4">
         <v>22.6</v>
       </c>
-      <c r="O67" s="5">
+      <c r="M67" s="4">
         <v>22.9</v>
       </c>
-      <c r="P67" s="5">
-        <v>23.2</v>
-      </c>
-      <c r="Q67" s="5">
+      <c r="N67" s="4">
+        <v>23.1</v>
+      </c>
+      <c r="O67" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="P67" s="4">
         <v>23.5</v>
       </c>
-      <c r="R67" s="5">
-        <v>23.8</v>
+      <c r="Q67" s="4">
+        <v>23.7</v>
+      </c>
+      <c r="R67" s="4">
+        <v>23.9</v>
       </c>
     </row>
     <row r="68" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3267,37 +3268,37 @@
       <c r="G68" s="5">
         <v>20.7</v>
       </c>
-      <c r="H68" s="5">
-        <v>21</v>
-      </c>
-      <c r="I68" s="5">
-        <v>21.3</v>
-      </c>
-      <c r="J68" s="5">
-        <v>21.6</v>
-      </c>
-      <c r="K68" s="5">
-        <v>21.9</v>
-      </c>
-      <c r="L68" s="5">
-        <v>22.2</v>
-      </c>
-      <c r="M68" s="5">
-        <v>22.5</v>
-      </c>
-      <c r="N68" s="5">
-        <v>22.8</v>
-      </c>
-      <c r="O68" s="5">
-        <v>23.1</v>
-      </c>
-      <c r="P68" s="5">
+      <c r="H68" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="I68" s="4">
+        <v>21.8</v>
+      </c>
+      <c r="J68" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="K68" s="4">
+        <v>22.4</v>
+      </c>
+      <c r="L68" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="M68" s="4">
+        <v>23</v>
+      </c>
+      <c r="N68" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="O68" s="4">
         <v>23.4</v>
       </c>
-      <c r="Q68" s="5">
-        <v>23.7</v>
-      </c>
-      <c r="R68" s="5">
+      <c r="P68" s="4">
+        <v>23.6</v>
+      </c>
+      <c r="Q68" s="4">
+        <v>23.8</v>
+      </c>
+      <c r="R68" s="4">
         <v>24</v>
       </c>
     </row>

</xml_diff>